<commit_message>
Updated Excel Lines-of-Code graph
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2 - 2_1_0/Fotogroep Waalre/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C32AF3-1306-7F47-B3C1-CDF59D1673BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FBB0FB-FFA3-4843-B8FA-287F4E63371F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30160" windowHeight="26560" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30160" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -205,7 +205,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -559,6 +559,9 @@
                 <c:pt idx="96">
                   <c:v>44709</c:v>
                 </c:pt>
+                <c:pt idx="97">
+                  <c:v>44781</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -858,6 +861,9 @@
                 </c:pt>
                 <c:pt idx="96">
                   <c:v>3817</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3886</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -873,10 +879,10 @@
           <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Code</c:v>
+            <c:v>Swift code</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="44450" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -1196,6 +1202,9 @@
                 <c:pt idx="96">
                   <c:v>44709</c:v>
                 </c:pt>
+                <c:pt idx="97">
+                  <c:v>44781</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1495,6 +1504,9 @@
                 </c:pt>
                 <c:pt idx="96">
                   <c:v>3023</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3079</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1513,7 +1525,7 @@
             <c:v>Comments</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="6350" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
@@ -1835,6 +1847,9 @@
                 <c:pt idx="96">
                   <c:v>44709</c:v>
                 </c:pt>
+                <c:pt idx="97">
+                  <c:v>44781</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2134,6 +2149,9 @@
                 </c:pt>
                 <c:pt idx="96">
                   <c:v>417</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>423</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2152,7 +2170,7 @@
             <c:v>Blank lines</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="50000"/>
@@ -2209,7 +2227,7 @@
             </c:marker>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:ln w="6350" cap="rnd">
+              <a:ln w="25400" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="50000"/>
@@ -2523,6 +2541,9 @@
                 <c:pt idx="96">
                   <c:v>44709</c:v>
                 </c:pt>
+                <c:pt idx="97">
+                  <c:v>44781</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2822,6 +2843,9 @@
                 </c:pt>
                 <c:pt idx="96">
                   <c:v>377</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>384</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2848,7 +2872,7 @@
         <c:axId val="1582352671"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="44750"/>
+          <c:max val="44850"/>
           <c:min val="44349"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2914,7 +2938,7 @@
         <c:axId val="1582338719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="4000"/>
+          <c:max val="4500"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3056,8 +3080,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1054842261614604"/>
-          <c:y val="6.4535827711273586E-2"/>
+          <c:x val="0.6393516697157211"/>
+          <c:y val="0.59630513927694528"/>
           <c:w val="8.6045271289377251E-2"/>
           <c:h val="0.14401330501945014"/>
         </c:manualLayout>
@@ -4031,13 +4055,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K99"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B43" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N89" sqref="N89"/>
+      <selection pane="bottomRight" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7713,7 +7737,7 @@
         <v>36</v>
       </c>
       <c r="H99" s="18">
-        <f t="shared" ref="H99" si="119">SUM(I99:K99)</f>
+        <f t="shared" ref="H99:H100" si="119">SUM(I99:K99)</f>
         <v>3817</v>
       </c>
       <c r="I99" s="6">
@@ -7724,6 +7748,43 @@
       </c>
       <c r="K99" s="8">
         <v>377</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>44781</v>
+      </c>
+      <c r="B100" s="2">
+        <v>9</v>
+      </c>
+      <c r="C100" s="3">
+        <f t="shared" ref="C100" si="120">SUM(D100:F100)</f>
+        <v>1673</v>
+      </c>
+      <c r="D100" s="3">
+        <v>1105</v>
+      </c>
+      <c r="E100" s="3">
+        <v>371</v>
+      </c>
+      <c r="F100" s="4">
+        <v>197</v>
+      </c>
+      <c r="G100" s="5">
+        <v>39</v>
+      </c>
+      <c r="H100" s="18">
+        <f t="shared" si="119"/>
+        <v>3886</v>
+      </c>
+      <c r="I100" s="6">
+        <v>3079</v>
+      </c>
+      <c r="J100" s="7">
+        <v>423</v>
+      </c>
+      <c r="K100" s="8">
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -7743,8 +7804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W37" sqref="W37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Disabled text autocorrection on Search field.
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FBB0FB-FFA3-4843-B8FA-287F4E63371F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61063E63-63DD-0F4E-9995-9118378A7792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30160" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -264,10 +264,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Table!$A$3:$A$100</c:f>
+              <c:f>Table!$A$3:$A$150</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="98"/>
+                <c:ptCount val="148"/>
                 <c:pt idx="0">
                   <c:v>44380</c:v>
                 </c:pt>
@@ -561,16 +561,22 @@
                 </c:pt>
                 <c:pt idx="97">
                   <c:v>44781</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>44785</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>44787</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Table!$H$3:$H$100</c:f>
+              <c:f>Table!$H$3:$H$150</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="98"/>
+                <c:ptCount val="148"/>
                 <c:pt idx="0">
                   <c:v>340</c:v>
                 </c:pt>
@@ -864,6 +870,12 @@
                 </c:pt>
                 <c:pt idx="97">
                   <c:v>3886</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3890</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -907,10 +919,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Table!$A$3:$A$100</c:f>
+              <c:f>Table!$A$3:$A$150</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="98"/>
+                <c:ptCount val="148"/>
                 <c:pt idx="0">
                   <c:v>44380</c:v>
                 </c:pt>
@@ -1204,16 +1216,22 @@
                 </c:pt>
                 <c:pt idx="97">
                   <c:v>44781</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>44785</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>44787</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Table!$I$3:$I$100</c:f>
+              <c:f>Table!$I$3:$I$150</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="98"/>
+                <c:ptCount val="148"/>
                 <c:pt idx="0">
                   <c:v>239</c:v>
                 </c:pt>
@@ -1507,6 +1525,12 @@
                 </c:pt>
                 <c:pt idx="97">
                   <c:v>3079</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3083</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3084</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1552,10 +1576,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Table!$A$3:$A$100</c:f>
+              <c:f>Table!$A$3:$A$150</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="98"/>
+                <c:ptCount val="148"/>
                 <c:pt idx="0">
                   <c:v>44380</c:v>
                 </c:pt>
@@ -1849,16 +1873,22 @@
                 </c:pt>
                 <c:pt idx="97">
                   <c:v>44781</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>44785</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>44787</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Table!$J$3:$J$100</c:f>
+              <c:f>Table!$J$3:$J$150</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="98"/>
+                <c:ptCount val="148"/>
                 <c:pt idx="0">
                   <c:v>61</c:v>
                 </c:pt>
@@ -2151,6 +2181,12 @@
                   <c:v>417</c:v>
                 </c:pt>
                 <c:pt idx="97">
+                  <c:v>423</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>423</c:v>
+                </c:pt>
+                <c:pt idx="99">
                   <c:v>423</c:v>
                 </c:pt>
               </c:numCache>
@@ -2246,10 +2282,10 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>Table!$A$3:$A$100</c:f>
+              <c:f>Table!$A$3:$A$150</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="98"/>
+                <c:ptCount val="148"/>
                 <c:pt idx="0">
                   <c:v>44380</c:v>
                 </c:pt>
@@ -2543,16 +2579,22 @@
                 </c:pt>
                 <c:pt idx="97">
                   <c:v>44781</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>44785</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>44787</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Table!$K$3:$K$100</c:f>
+              <c:f>Table!$K$3:$K$150</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="98"/>
+                <c:ptCount val="148"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
@@ -2845,6 +2887,12 @@
                   <c:v>377</c:v>
                 </c:pt>
                 <c:pt idx="97">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="99">
                   <c:v>384</c:v>
                 </c:pt>
               </c:numCache>
@@ -4055,13 +4103,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K100"/>
+  <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M12" sqref="M12"/>
+      <selection pane="bottomRight" activeCell="K102" sqref="K102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7737,7 +7785,7 @@
         <v>36</v>
       </c>
       <c r="H99" s="18">
-        <f t="shared" ref="H99:H100" si="119">SUM(I99:K99)</f>
+        <f t="shared" ref="H99:H102" si="119">SUM(I99:K99)</f>
         <v>3817</v>
       </c>
       <c r="I99" s="6">
@@ -7784,6 +7832,80 @@
         <v>423</v>
       </c>
       <c r="K100" s="8">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>44785</v>
+      </c>
+      <c r="B101" s="2">
+        <v>9</v>
+      </c>
+      <c r="C101" s="3">
+        <f t="shared" ref="C101" si="121">SUM(D101:F101)</f>
+        <v>1673</v>
+      </c>
+      <c r="D101" s="3">
+        <v>1105</v>
+      </c>
+      <c r="E101" s="3">
+        <v>371</v>
+      </c>
+      <c r="F101" s="4">
+        <v>197</v>
+      </c>
+      <c r="G101" s="5">
+        <v>39</v>
+      </c>
+      <c r="H101" s="18">
+        <f t="shared" si="119"/>
+        <v>3890</v>
+      </c>
+      <c r="I101" s="6">
+        <v>3083</v>
+      </c>
+      <c r="J101" s="7">
+        <v>423</v>
+      </c>
+      <c r="K101" s="8">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>44787</v>
+      </c>
+      <c r="B102" s="2">
+        <v>9</v>
+      </c>
+      <c r="C102" s="3">
+        <f t="shared" ref="C102" si="122">SUM(D102:F102)</f>
+        <v>1673</v>
+      </c>
+      <c r="D102" s="3">
+        <v>1105</v>
+      </c>
+      <c r="E102" s="3">
+        <v>371</v>
+      </c>
+      <c r="F102" s="4">
+        <v>197</v>
+      </c>
+      <c r="G102" s="5">
+        <v>39</v>
+      </c>
+      <c r="H102" s="18">
+        <f t="shared" si="119"/>
+        <v>3891</v>
+      </c>
+      <c r="I102" s="6">
+        <v>3084</v>
+      </c>
+      <c r="J102" s="7">
+        <v>423</v>
+      </c>
+      <c r="K102" s="8">
         <v>384</v>
       </c>
     </row>
@@ -7805,7 +7927,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+      <selection activeCell="W33" sqref="W33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Refactored names of Views and their file names.
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61063E63-63DD-0F4E-9995-9118378A7792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0139C208-327B-4C4C-AA57-CF78BDD3127D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30160" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -568,6 +568,9 @@
                 <c:pt idx="99">
                   <c:v>44787</c:v>
                 </c:pt>
+                <c:pt idx="100">
+                  <c:v>44808</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -876,6 +879,9 @@
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>3891</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>3906</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1223,6 +1229,9 @@
                 <c:pt idx="99">
                   <c:v>44787</c:v>
                 </c:pt>
+                <c:pt idx="100">
+                  <c:v>44808</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1531,6 +1540,9 @@
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>3084</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>3098</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1880,6 +1892,9 @@
                 <c:pt idx="99">
                   <c:v>44787</c:v>
                 </c:pt>
+                <c:pt idx="100">
+                  <c:v>44808</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2188,6 +2203,9 @@
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>423</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>425</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2586,6 +2604,9 @@
                 <c:pt idx="99">
                   <c:v>44787</c:v>
                 </c:pt>
+                <c:pt idx="100">
+                  <c:v>44808</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2894,6 +2915,9 @@
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>383</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4103,13 +4127,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K102"/>
+  <dimension ref="A1:K103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K102" sqref="K102"/>
+      <selection pane="bottomRight" activeCell="I103" sqref="I103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7907,6 +7931,43 @@
       </c>
       <c r="K102" s="8">
         <v>384</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>44808</v>
+      </c>
+      <c r="B103" s="2">
+        <v>9</v>
+      </c>
+      <c r="C103" s="3">
+        <f t="shared" ref="C103" si="123">SUM(D103:F103)</f>
+        <v>1673</v>
+      </c>
+      <c r="D103" s="3">
+        <v>1105</v>
+      </c>
+      <c r="E103" s="3">
+        <v>371</v>
+      </c>
+      <c r="F103" s="4">
+        <v>197</v>
+      </c>
+      <c r="G103" s="5">
+        <v>39</v>
+      </c>
+      <c r="H103" s="18">
+        <f t="shared" ref="H103" si="124">SUM(I103:K103)</f>
+        <v>3906</v>
+      </c>
+      <c r="I103" s="6">
+        <v>3098</v>
+      </c>
+      <c r="J103" s="7">
+        <v>425</v>
+      </c>
+      <c r="K103" s="8">
+        <v>383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Documentation and print() statements
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0139C208-327B-4C4C-AA57-CF78BDD3127D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648F0B91-19E3-934D-8136-A68D8385EC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30160" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -881,7 +881,7 @@
                   <c:v>3891</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>3906</c:v>
+                  <c:v>3909</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1542,7 +1542,7 @@
                   <c:v>3084</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>3098</c:v>
+                  <c:v>3104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2205,7 +2205,7 @@
                   <c:v>423</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>425</c:v>
+                  <c:v>423</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2917,7 +2917,7 @@
                   <c:v>384</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>383</c:v>
+                  <c:v>382</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4133,7 +4133,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I103" sqref="I103"/>
+      <selection pane="bottomRight" activeCell="I104" sqref="I104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7958,16 +7958,16 @@
       </c>
       <c r="H103" s="18">
         <f t="shared" ref="H103" si="124">SUM(I103:K103)</f>
-        <v>3906</v>
+        <v>3909</v>
       </c>
       <c r="I103" s="6">
-        <v>3098</v>
+        <v>3104</v>
       </c>
       <c r="J103" s="7">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="K103" s="8">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update line count FotoGroupWaalre.xls
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6671B16-DE7F-A04A-869F-217B4F979C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C46605-A9AB-6F4D-814E-B8B6756ABF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30160" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -580,6 +580,9 @@
                 <c:pt idx="103">
                   <c:v>44815</c:v>
                 </c:pt>
+                <c:pt idx="104">
+                  <c:v>44821</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -900,6 +903,9 @@
                 </c:pt>
                 <c:pt idx="103">
                   <c:v>3973</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>3873</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1259,6 +1265,9 @@
                 <c:pt idx="103">
                   <c:v>44815</c:v>
                 </c:pt>
+                <c:pt idx="104">
+                  <c:v>44821</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1579,6 +1588,9 @@
                 </c:pt>
                 <c:pt idx="103">
                   <c:v>3163</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>3069</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1940,6 +1952,9 @@
                 <c:pt idx="103">
                   <c:v>44815</c:v>
                 </c:pt>
+                <c:pt idx="104">
+                  <c:v>44821</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2259,6 +2274,9 @@
                   <c:v>422</c:v>
                 </c:pt>
                 <c:pt idx="103">
+                  <c:v>423</c:v>
+                </c:pt>
+                <c:pt idx="104">
                   <c:v>423</c:v>
                 </c:pt>
               </c:numCache>
@@ -2670,6 +2688,9 @@
                 <c:pt idx="103">
                   <c:v>44815</c:v>
                 </c:pt>
+                <c:pt idx="104">
+                  <c:v>44821</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2990,6 +3011,9 @@
                 </c:pt>
                 <c:pt idx="103">
                   <c:v>387</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>381</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4199,13 +4223,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K106"/>
+  <dimension ref="A1:K107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I107" sqref="I107"/>
+      <selection pane="bottomRight" activeCell="I108" sqref="I108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8151,6 +8175,43 @@
       </c>
       <c r="K106" s="8">
         <v>387</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>44821</v>
+      </c>
+      <c r="B107" s="2">
+        <v>9</v>
+      </c>
+      <c r="C107" s="3">
+        <f t="shared" ref="C107" si="131">SUM(D107:F107)</f>
+        <v>1673</v>
+      </c>
+      <c r="D107" s="3">
+        <v>1105</v>
+      </c>
+      <c r="E107" s="3">
+        <v>371</v>
+      </c>
+      <c r="F107" s="4">
+        <v>197</v>
+      </c>
+      <c r="G107" s="5">
+        <v>39</v>
+      </c>
+      <c r="H107" s="18">
+        <f t="shared" ref="H107" si="132">SUM(I107:K107)</f>
+        <v>3873</v>
+      </c>
+      <c r="I107" s="6">
+        <v>3069</v>
+      </c>
+      <c r="J107" s="7">
+        <v>423</v>
+      </c>
+      <c r="K107" s="8">
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated line count stats
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C46605-A9AB-6F4D-814E-B8B6756ABF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECF813C-1DE0-994B-9EC9-C71FC86249F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30160" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30160" windowHeight="26560" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -583,6 +583,9 @@
                 <c:pt idx="104">
                   <c:v>44821</c:v>
                 </c:pt>
+                <c:pt idx="105">
+                  <c:v>44823</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -905,6 +908,9 @@
                   <c:v>3973</c:v>
                 </c:pt>
                 <c:pt idx="104">
+                  <c:v>3873</c:v>
+                </c:pt>
+                <c:pt idx="105">
                   <c:v>3873</c:v>
                 </c:pt>
               </c:numCache>
@@ -1268,6 +1274,9 @@
                 <c:pt idx="104">
                   <c:v>44821</c:v>
                 </c:pt>
+                <c:pt idx="105">
+                  <c:v>44823</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1590,6 +1599,9 @@
                   <c:v>3163</c:v>
                 </c:pt>
                 <c:pt idx="104">
+                  <c:v>3069</c:v>
+                </c:pt>
+                <c:pt idx="105">
                   <c:v>3069</c:v>
                 </c:pt>
               </c:numCache>
@@ -1955,6 +1967,9 @@
                 <c:pt idx="104">
                   <c:v>44821</c:v>
                 </c:pt>
+                <c:pt idx="105">
+                  <c:v>44823</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2277,6 +2292,9 @@
                   <c:v>423</c:v>
                 </c:pt>
                 <c:pt idx="104">
+                  <c:v>423</c:v>
+                </c:pt>
+                <c:pt idx="105">
                   <c:v>423</c:v>
                 </c:pt>
               </c:numCache>
@@ -2691,6 +2709,9 @@
                 <c:pt idx="104">
                   <c:v>44821</c:v>
                 </c:pt>
+                <c:pt idx="105">
+                  <c:v>44823</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3013,6 +3034,9 @@
                   <c:v>387</c:v>
                 </c:pt>
                 <c:pt idx="104">
+                  <c:v>381</c:v>
+                </c:pt>
+                <c:pt idx="105">
                   <c:v>381</c:v>
                 </c:pt>
               </c:numCache>
@@ -4223,13 +4247,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K107"/>
+  <dimension ref="A1:K108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I108" sqref="I108"/>
+      <selection pane="bottomRight" activeCell="I109" sqref="I109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8214,6 +8238,43 @@
         <v>381</v>
       </c>
     </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>44823</v>
+      </c>
+      <c r="B108" s="2">
+        <v>9</v>
+      </c>
+      <c r="C108" s="3">
+        <f t="shared" ref="C108" si="133">SUM(D108:F108)</f>
+        <v>1673</v>
+      </c>
+      <c r="D108" s="3">
+        <v>1105</v>
+      </c>
+      <c r="E108" s="3">
+        <v>371</v>
+      </c>
+      <c r="F108" s="4">
+        <v>197</v>
+      </c>
+      <c r="G108" s="5">
+        <v>39</v>
+      </c>
+      <c r="H108" s="18">
+        <f t="shared" ref="H108" si="134">SUM(I108:K108)</f>
+        <v>3873</v>
+      </c>
+      <c r="I108" s="6">
+        <v>3069</v>
+      </c>
+      <c r="J108" s="7">
+        <v>423</v>
+      </c>
+      <c r="K108" s="8">
+        <v>381</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:F1"/>
@@ -8231,7 +8292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W33" sqref="W33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Delete photo club feature
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5820B3F3-791E-F64A-AB5E-DCAA031296ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6D695C-A764-C645-974D-23928C19F30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30160" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -589,6 +589,9 @@
                 <c:pt idx="106">
                   <c:v>44824</c:v>
                 </c:pt>
+                <c:pt idx="107">
+                  <c:v>44829</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -918,6 +921,9 @@
                 </c:pt>
                 <c:pt idx="106">
                   <c:v>3999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>4032</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1286,6 +1292,9 @@
                 <c:pt idx="106">
                   <c:v>44824</c:v>
                 </c:pt>
+                <c:pt idx="107">
+                  <c:v>44829</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1615,6 +1624,9 @@
                 </c:pt>
                 <c:pt idx="106">
                   <c:v>3161</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>3185</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1985,6 +1997,9 @@
                 <c:pt idx="106">
                   <c:v>44824</c:v>
                 </c:pt>
+                <c:pt idx="107">
+                  <c:v>44829</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2314,6 +2329,9 @@
                 </c:pt>
                 <c:pt idx="106">
                   <c:v>449</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>459</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2733,6 +2751,9 @@
                 <c:pt idx="106">
                   <c:v>44824</c:v>
                 </c:pt>
+                <c:pt idx="107">
+                  <c:v>44829</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3062,6 +3083,9 @@
                 </c:pt>
                 <c:pt idx="106">
                   <c:v>389</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>388</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4271,13 +4295,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K109"/>
+  <dimension ref="A1:K110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I110" sqref="I110"/>
+      <selection pane="bottomRight" activeCell="I111" sqref="I111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8334,6 +8358,43 @@
       </c>
       <c r="K109" s="8">
         <v>389</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>44829</v>
+      </c>
+      <c r="B110" s="2">
+        <v>9</v>
+      </c>
+      <c r="C110" s="3">
+        <f t="shared" ref="C110" si="137">SUM(D110:F110)</f>
+        <v>1673</v>
+      </c>
+      <c r="D110" s="3">
+        <v>1105</v>
+      </c>
+      <c r="E110" s="3">
+        <v>371</v>
+      </c>
+      <c r="F110" s="4">
+        <v>197</v>
+      </c>
+      <c r="G110" s="5">
+        <v>39</v>
+      </c>
+      <c r="H110" s="18">
+        <f t="shared" ref="H110" si="138">SUM(I110:K110)</f>
+        <v>4032</v>
+      </c>
+      <c r="I110" s="6">
+        <v>3185</v>
+      </c>
+      <c r="J110" s="7">
+        <v>459</v>
+      </c>
+      <c r="K110" s="8">
+        <v>388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated line count graph
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6D695C-A764-C645-974D-23928C19F30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E965975-EA27-8F4D-A979-8B613BA021BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30160" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -592,6 +592,9 @@
                 <c:pt idx="107">
                   <c:v>44829</c:v>
                 </c:pt>
+                <c:pt idx="108">
+                  <c:v>44842</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -924,6 +927,9 @@
                 </c:pt>
                 <c:pt idx="107">
                   <c:v>4032</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>4157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1295,6 +1301,9 @@
                 <c:pt idx="107">
                   <c:v>44829</c:v>
                 </c:pt>
+                <c:pt idx="108">
+                  <c:v>44842</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1627,6 +1636,9 @@
                 </c:pt>
                 <c:pt idx="107">
                   <c:v>3185</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>3297</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2000,6 +2012,9 @@
                 <c:pt idx="107">
                   <c:v>44829</c:v>
                 </c:pt>
+                <c:pt idx="108">
+                  <c:v>44842</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2332,6 +2347,9 @@
                 </c:pt>
                 <c:pt idx="107">
                   <c:v>459</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>457</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2754,6 +2772,9 @@
                 <c:pt idx="107">
                   <c:v>44829</c:v>
                 </c:pt>
+                <c:pt idx="108">
+                  <c:v>44842</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3086,6 +3107,9 @@
                 </c:pt>
                 <c:pt idx="107">
                   <c:v>388</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>403</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4295,13 +4319,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K110"/>
+  <dimension ref="A1:K111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I111" sqref="I111"/>
+      <selection pane="bottomRight" activeCell="I112" sqref="I112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8395,6 +8419,43 @@
       </c>
       <c r="K110" s="8">
         <v>388</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <v>44842</v>
+      </c>
+      <c r="B111" s="2">
+        <v>9</v>
+      </c>
+      <c r="C111" s="3">
+        <f t="shared" ref="C111" si="139">SUM(D111:F111)</f>
+        <v>1673</v>
+      </c>
+      <c r="D111" s="3">
+        <v>1105</v>
+      </c>
+      <c r="E111" s="3">
+        <v>371</v>
+      </c>
+      <c r="F111" s="4">
+        <v>197</v>
+      </c>
+      <c r="G111" s="5">
+        <v>39</v>
+      </c>
+      <c r="H111" s="18">
+        <f t="shared" ref="H111" si="140">SUM(I111:K111)</f>
+        <v>4157</v>
+      </c>
+      <c r="I111" s="6">
+        <v>3297</v>
+      </c>
+      <c r="J111" s="7">
+        <v>457</v>
+      </c>
+      <c r="K111" s="8">
+        <v>403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed from MapPin to MapMarker on MapKit
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E965975-EA27-8F4D-A979-8B613BA021BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE87652-BB95-4441-881F-CDDB094D2501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30160" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -595,6 +595,9 @@
                 <c:pt idx="108">
                   <c:v>44842</c:v>
                 </c:pt>
+                <c:pt idx="109">
+                  <c:v>44846</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -930,6 +933,9 @@
                 </c:pt>
                 <c:pt idx="108">
                   <c:v>4157</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>4163</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1304,6 +1310,9 @@
                 <c:pt idx="108">
                   <c:v>44842</c:v>
                 </c:pt>
+                <c:pt idx="109">
+                  <c:v>44846</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1639,6 +1648,9 @@
                 </c:pt>
                 <c:pt idx="108">
                   <c:v>3297</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>3302</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2015,6 +2027,9 @@
                 <c:pt idx="108">
                   <c:v>44842</c:v>
                 </c:pt>
+                <c:pt idx="109">
+                  <c:v>44846</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2350,6 +2365,9 @@
                 </c:pt>
                 <c:pt idx="108">
                   <c:v>457</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>458</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2775,6 +2793,9 @@
                 <c:pt idx="108">
                   <c:v>44842</c:v>
                 </c:pt>
+                <c:pt idx="109">
+                  <c:v>44846</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3109,6 +3130,9 @@
                   <c:v>388</c:v>
                 </c:pt>
                 <c:pt idx="108">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="109">
                   <c:v>403</c:v>
                 </c:pt>
               </c:numCache>
@@ -4319,13 +4343,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K111"/>
+  <dimension ref="A1:K112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I112" sqref="I112"/>
+      <selection pane="bottomRight" activeCell="I113" sqref="I113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8455,6 +8479,43 @@
         <v>457</v>
       </c>
       <c r="K111" s="8">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <v>44846</v>
+      </c>
+      <c r="B112" s="2">
+        <v>9</v>
+      </c>
+      <c r="C112" s="3">
+        <f t="shared" ref="C112" si="141">SUM(D112:F112)</f>
+        <v>1673</v>
+      </c>
+      <c r="D112" s="3">
+        <v>1105</v>
+      </c>
+      <c r="E112" s="3">
+        <v>371</v>
+      </c>
+      <c r="F112" s="4">
+        <v>197</v>
+      </c>
+      <c r="G112" s="5">
+        <v>39</v>
+      </c>
+      <c r="H112" s="18">
+        <f t="shared" ref="H112" si="142">SUM(I112:K112)</f>
+        <v>4163</v>
+      </c>
+      <c r="I112" s="6">
+        <v>3302</v>
+      </c>
+      <c r="J112" s="7">
+        <v>458</v>
+      </c>
+      <c r="K112" s="8">
         <v>403</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Administration to start work of 2.2.3
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE87652-BB95-4441-881F-CDDB094D2501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B799BF-B75C-774A-B07B-F20D277B6562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30160" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -598,6 +598,9 @@
                 <c:pt idx="109">
                   <c:v>44846</c:v>
                 </c:pt>
+                <c:pt idx="110">
+                  <c:v>44857</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -936,6 +939,9 @@
                 </c:pt>
                 <c:pt idx="109">
                   <c:v>4163</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>4165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1313,6 +1319,9 @@
                 <c:pt idx="109">
                   <c:v>44846</c:v>
                 </c:pt>
+                <c:pt idx="110">
+                  <c:v>44857</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1651,6 +1660,9 @@
                 </c:pt>
                 <c:pt idx="109">
                   <c:v>3302</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>3304</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2030,6 +2042,9 @@
                 <c:pt idx="109">
                   <c:v>44846</c:v>
                 </c:pt>
+                <c:pt idx="110">
+                  <c:v>44857</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2367,6 +2382,9 @@
                   <c:v>457</c:v>
                 </c:pt>
                 <c:pt idx="109">
+                  <c:v>458</c:v>
+                </c:pt>
+                <c:pt idx="110">
                   <c:v>458</c:v>
                 </c:pt>
               </c:numCache>
@@ -2796,6 +2814,9 @@
                 <c:pt idx="109">
                   <c:v>44846</c:v>
                 </c:pt>
+                <c:pt idx="110">
+                  <c:v>44857</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3133,6 +3154,9 @@
                   <c:v>403</c:v>
                 </c:pt>
                 <c:pt idx="109">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="110">
                   <c:v>403</c:v>
                 </c:pt>
               </c:numCache>
@@ -3160,7 +3184,7 @@
         <c:axId val="1582352671"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="44850"/>
+          <c:max val="44900"/>
           <c:min val="44349"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4013,8 +4037,8 @@
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -4343,13 +4367,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K112"/>
+  <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I113" sqref="I113"/>
+      <selection pane="bottomRight" activeCell="I114" sqref="I114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8516,6 +8540,43 @@
         <v>458</v>
       </c>
       <c r="K112" s="8">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <v>44857</v>
+      </c>
+      <c r="B113" s="2">
+        <v>9</v>
+      </c>
+      <c r="C113" s="3">
+        <f t="shared" ref="C113" si="143">SUM(D113:F113)</f>
+        <v>1673</v>
+      </c>
+      <c r="D113" s="3">
+        <v>1105</v>
+      </c>
+      <c r="E113" s="3">
+        <v>371</v>
+      </c>
+      <c r="F113" s="4">
+        <v>197</v>
+      </c>
+      <c r="G113" s="5">
+        <v>39</v>
+      </c>
+      <c r="H113" s="18">
+        <f t="shared" ref="H113" si="144">SUM(I113:K113)</f>
+        <v>4165</v>
+      </c>
+      <c r="I113" s="6">
+        <v>3304</v>
+      </c>
+      <c r="J113" s="7">
+        <v>458</v>
+      </c>
+      <c r="K113" s="8">
         <v>403</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Administrative changes for future 2.2.4 release
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B799BF-B75C-774A-B07B-F20D277B6562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5850BF2-C08D-8B48-B5A8-4618107B7EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -241,6 +241,727 @@
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Table!$A$3:$A$150</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="148"/>
+                <c:pt idx="0">
+                  <c:v>44380</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44381</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44382</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44383</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44387</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44392</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44393</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44394</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44395</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44396</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44397</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44398</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44401</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44402</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44409</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44410</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44415</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44416</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44417</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44422</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44423</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44424</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44425</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44472</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44539</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44541</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44542</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44547</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44549</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44550</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44551</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44552</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44553</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44554</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44555</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44556</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44558</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44559</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44560</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44561</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44564</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44565</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44566</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44567</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44568</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44569</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44575</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44576</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44577</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44578</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>44579</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44584</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>44585</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>44586</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44587</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>44588</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44589</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>44590</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>44626</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>44627</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>44628</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>44632</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>44633</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>44637</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>44644</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>44645</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>44646</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>44647</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>44648</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>44651</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>44653</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>44654</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>44655</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>44656</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>44661</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>44663</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>44668</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>44669</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>44672</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>44674</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>44675</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>44678</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>44686</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>44688</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>44689</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>44690</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>44698</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>44700</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>44701</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>44702</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>44707</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>44709</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>44781</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>44785</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>44787</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>44808</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>44812</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>44814</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>44815</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>44821</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>44823</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>44824</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>44829</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>44842</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>44846</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>44857</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Table!$H$3:$H$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="148"/>
+                <c:pt idx="0">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>551</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>642</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>684</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>695</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>714</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>717</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1173</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1171</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1187</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1197</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1213</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1223</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1241</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1296</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1332</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1335</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1338</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1375</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1372</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1417</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1414</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1921</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1920</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1717</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1703</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1737</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1760</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1769</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1817</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1838</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1837</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1848</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1896</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1905</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1924</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2105</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2209</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2209</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2221</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2221</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2293</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2320</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2449</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2518</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2567</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2927</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2915</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2917</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2862</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2949</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2976</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3025</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3025</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3027</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3029</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2686</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3024</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3031</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3033</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3053</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3057</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3090</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3109</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3126</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3277</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3287</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3284</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3331</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3333</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3450</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3465</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3489</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3496</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3526</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3558</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3526</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3891</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3908</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3763</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3744</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3752</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>3704</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3691</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3719</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3694</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3710</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3727</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3721</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3721</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3799</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3817</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3886</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3890</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3891</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>3909</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>3930</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>3943</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>3973</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>3873</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>3873</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>3999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>4032</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>4157</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>4163</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>4180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-207B-2046-BDBA-43068CA74D1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Swift code</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
@@ -252,7 +973,7 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="bg1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
@@ -606,727 +1327,6 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Table!$H$3:$H$150</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="148"/>
-                <c:pt idx="0">
-                  <c:v>340</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>551</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>630</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>642</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>684</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>695</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>714</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>717</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1173</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1171</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1187</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1197</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1213</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1223</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1241</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1296</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1332</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1335</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1338</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1375</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1372</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1417</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1414</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1921</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1920</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1717</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1703</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1737</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1760</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1769</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1817</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1838</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1837</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1848</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1896</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1905</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1924</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2035</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2022</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2105</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2209</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2209</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2221</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>2221</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>2293</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2320</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>2449</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>2518</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>2567</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>2927</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>2915</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>2917</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>2862</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>2949</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>2976</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>3025</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>3025</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>3027</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>3029</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>2686</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>3024</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>3031</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>3033</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>3053</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>3057</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>3090</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>3109</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>3126</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>3277</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>3287</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>3284</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>3331</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>3333</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>3450</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>3465</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>3489</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>3496</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>3526</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>3558</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>3526</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>3891</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>3908</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>3763</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>3744</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>3752</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>3704</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>3691</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>3719</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>3694</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>3700</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>3710</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>3727</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>3721</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>3721</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>3799</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>3817</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>3886</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>3890</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>3891</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>3909</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>3930</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>3943</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>3973</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>3873</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>3873</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>3999</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>4032</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>4157</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>4163</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>4165</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-207B-2046-BDBA-43068CA74D1D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Swift code</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Table!$A$3:$A$150</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="148"/>
-                <c:pt idx="0">
-                  <c:v>44380</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>44381</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>44382</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>44383</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>44384</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>44387</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>44392</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44393</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44394</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44395</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44396</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>44397</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>44398</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>44400</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>44401</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>44402</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>44409</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>44410</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>44415</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>44416</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>44417</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>44422</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44423</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>44424</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>44425</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>44472</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>44539</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>44541</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>44542</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>44547</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>44549</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>44550</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>44551</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>44552</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>44553</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>44554</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>44555</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>44556</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>44558</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>44559</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>44560</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>44561</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>44562</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>44564</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>44565</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>44566</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>44567</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>44568</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>44569</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>44575</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>44576</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>44577</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>44578</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>44579</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>44584</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>44585</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>44586</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>44587</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>44588</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>44589</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>44590</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>44626</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>44627</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>44628</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>44632</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>44633</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>44637</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>44644</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>44645</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>44646</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>44647</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>44648</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>44651</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>44652</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>44653</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>44654</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>44655</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>44656</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>44661</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>44663</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>44668</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>44669</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>44672</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>44674</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>44675</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>44678</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>44682</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>44686</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>44688</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>44689</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>44690</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>44698</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>44700</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>44701</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>44702</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>44707</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>44709</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>44781</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>44785</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>44787</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>44808</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>44812</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>44814</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>44815</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>44821</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>44823</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>44824</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>44829</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>44842</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>44846</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>44857</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
               <c:f>Table!$I$3:$I$150</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
@@ -1662,12 +1662,12 @@
                   <c:v>3302</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>3304</c:v>
+                  <c:v>3319</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-207B-2046-BDBA-43068CA74D1D}"/>
@@ -1694,7 +1694,7 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="bg1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
@@ -2390,7 +2390,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-207B-2046-BDBA-43068CA74D1D}"/>
@@ -2406,10 +2406,7 @@
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2420,17 +2417,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
+                <a:schemeClr val="bg1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent4"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2443,17 +2434,11 @@
               <c:size val="5"/>
               <c:spPr>
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="bg1"/>
                 </a:solidFill>
                 <a:ln w="9525">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="50000"/>
-                      <a:lumOff val="50000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="accent4"/>
                   </a:solidFill>
                 </a:ln>
                 <a:effectLst/>
@@ -2463,10 +2448,7 @@
             <c:spPr>
               <a:ln w="25400" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent4"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
@@ -3162,7 +3144,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-207B-2046-BDBA-43068CA74D1D}"/>
@@ -3184,14 +3166,14 @@
         <c:axId val="1582352671"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="44900"/>
+          <c:max val="44930"/>
           <c:min val="44349"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="22225" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -3381,9 +3363,17 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="tx2"/>
+          </a:solidFill>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
       </c:spPr>
     </c:plotArea>
     <c:legend>
@@ -3400,11 +3390,21 @@
       </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
       </c:spPr>
       <c:txPr>
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -4373,7 +4373,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I114" sqref="I114"/>
+      <selection pane="bottomRight" activeCell="L113" sqref="L113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8568,10 +8568,10 @@
       </c>
       <c r="H113" s="18">
         <f t="shared" ref="H113" si="144">SUM(I113:K113)</f>
-        <v>4165</v>
+        <v>4180</v>
       </c>
       <c r="I113" s="6">
-        <v>3304</v>
+        <v>3319</v>
       </c>
       <c r="J113" s="7">
         <v>458</v>

</xml_diff>

<commit_message>
Updated line count spreadsheet
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre/Fotogroep Waalre/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5850BF2-C08D-8B48-B5A8-4618107B7EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7A10CA-F2A3-074F-A55E-08ADDE8AF789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -601,6 +601,9 @@
                 <c:pt idx="110">
                   <c:v>44857</c:v>
                 </c:pt>
+                <c:pt idx="111">
+                  <c:v>44892</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -942,6 +945,9 @@
                 </c:pt>
                 <c:pt idx="110">
                   <c:v>4180</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>4018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1322,6 +1328,9 @@
                 <c:pt idx="110">
                   <c:v>44857</c:v>
                 </c:pt>
+                <c:pt idx="111">
+                  <c:v>44892</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1663,6 +1672,9 @@
                 </c:pt>
                 <c:pt idx="110">
                   <c:v>3319</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>3221</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2045,6 +2057,9 @@
                 <c:pt idx="110">
                   <c:v>44857</c:v>
                 </c:pt>
+                <c:pt idx="111">
+                  <c:v>44892</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2386,6 +2401,9 @@
                 </c:pt>
                 <c:pt idx="110">
                   <c:v>458</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>413</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2799,6 +2817,9 @@
                 <c:pt idx="110">
                   <c:v>44857</c:v>
                 </c:pt>
+                <c:pt idx="111">
+                  <c:v>44892</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3140,6 +3161,9 @@
                 </c:pt>
                 <c:pt idx="110">
                   <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>384</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4367,13 +4391,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K113"/>
+  <dimension ref="A1:K114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L113" sqref="L113"/>
+      <selection pane="bottomRight" activeCell="I115" sqref="I115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8580,6 +8604,43 @@
         <v>403</v>
       </c>
     </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <v>44892</v>
+      </c>
+      <c r="B114" s="2">
+        <v>9</v>
+      </c>
+      <c r="C114" s="3">
+        <f t="shared" ref="C114" si="145">SUM(D114:F114)</f>
+        <v>1673</v>
+      </c>
+      <c r="D114" s="3">
+        <v>1105</v>
+      </c>
+      <c r="E114" s="3">
+        <v>371</v>
+      </c>
+      <c r="F114" s="4">
+        <v>197</v>
+      </c>
+      <c r="G114" s="5">
+        <v>39</v>
+      </c>
+      <c r="H114" s="18">
+        <f t="shared" ref="H114" si="146">SUM(I114:K114)</f>
+        <v>4018</v>
+      </c>
+      <c r="I114" s="6">
+        <v>3221</v>
+      </c>
+      <c r="J114" s="7">
+        <v>413</v>
+      </c>
+      <c r="K114" s="8">
+        <v>384</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:F1"/>
@@ -8598,7 +8659,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W33" sqref="W33"/>
+      <selection activeCell="AA41" sqref="AA41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Read birth date from online membership file for Fotogroep Waalre.
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7A10CA-F2A3-074F-A55E-08ADDE8AF789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7115F8FD-BBD2-3F41-96CF-7FDFD6C71990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -604,6 +604,9 @@
                 <c:pt idx="111">
                   <c:v>44892</c:v>
                 </c:pt>
+                <c:pt idx="112">
+                  <c:v>44899</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -948,6 +951,9 @@
                 </c:pt>
                 <c:pt idx="111">
                   <c:v>4018</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>4079</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1331,6 +1337,9 @@
                 <c:pt idx="111">
                   <c:v>44892</c:v>
                 </c:pt>
+                <c:pt idx="112">
+                  <c:v>44899</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1675,6 +1684,9 @@
                 </c:pt>
                 <c:pt idx="111">
                   <c:v>3221</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>3273</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2060,6 +2072,9 @@
                 <c:pt idx="111">
                   <c:v>44892</c:v>
                 </c:pt>
+                <c:pt idx="112">
+                  <c:v>44899</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2404,6 +2419,9 @@
                 </c:pt>
                 <c:pt idx="111">
                   <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2820,6 +2838,9 @@
                 <c:pt idx="111">
                   <c:v>44892</c:v>
                 </c:pt>
+                <c:pt idx="112">
+                  <c:v>44899</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3164,6 +3185,9 @@
                 </c:pt>
                 <c:pt idx="111">
                   <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>378</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4391,13 +4415,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K114"/>
+  <dimension ref="A1:K115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I115" sqref="I115"/>
+      <selection pane="bottomRight" activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8639,6 +8663,43 @@
       </c>
       <c r="K114" s="8">
         <v>384</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
+        <v>44899</v>
+      </c>
+      <c r="B115" s="2">
+        <v>9</v>
+      </c>
+      <c r="C115" s="3">
+        <f t="shared" ref="C115" si="147">SUM(D115:F115)</f>
+        <v>1673</v>
+      </c>
+      <c r="D115" s="3">
+        <v>1105</v>
+      </c>
+      <c r="E115" s="3">
+        <v>371</v>
+      </c>
+      <c r="F115" s="4">
+        <v>197</v>
+      </c>
+      <c r="G115" s="5">
+        <v>39</v>
+      </c>
+      <c r="H115" s="18">
+        <f t="shared" ref="H115" si="148">SUM(I115:K115)</f>
+        <v>4079</v>
+      </c>
+      <c r="I115" s="6">
+        <v>3273</v>
+      </c>
+      <c r="J115" s="7">
+        <v>428</v>
+      </c>
+      <c r="K115" s="8">
+        <v>378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extra param in getFileAsString() called okToUseEncryptedFile (for testing)
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7DF068-1BF1-D94A-BFCB-4C06A8A503A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC4F5FB-7080-CB4B-81F9-1DEBC4A46D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -960,7 +960,7 @@
                   <c:v>4089</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>4073</c:v>
+                  <c:v>4064</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1705,7 +1705,7 @@
                   <c:v>3282</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>3258</c:v>
+                  <c:v>3249</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4464,7 +4464,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I118" sqref="I118"/>
+      <selection pane="bottomRight" activeCell="K117" sqref="K117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8805,10 +8805,10 @@
       </c>
       <c r="H117">
         <f t="shared" ref="H117" si="152">SUM(I117:K117)</f>
-        <v>4073</v>
+        <v>4064</v>
       </c>
       <c r="I117" s="5">
-        <v>3258</v>
+        <v>3249</v>
       </c>
       <c r="J117" s="6">
         <v>434</v>

</xml_diff>

<commit_message>
Linecocunt based on NavigationStack branch
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD489D8F-E073-0446-A05F-E271FC38F4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A541561B-1D5B-3646-B736-248931D4D951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -611,6 +611,9 @@
                 <c:pt idx="115">
                   <c:v>44904</c:v>
                 </c:pt>
+                <c:pt idx="116">
+                  <c:v>44908</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -967,6 +970,9 @@
                 </c:pt>
                 <c:pt idx="115">
                   <c:v>4070</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>4054</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1362,6 +1368,9 @@
                 <c:pt idx="115">
                   <c:v>44904</c:v>
                 </c:pt>
+                <c:pt idx="116">
+                  <c:v>44908</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1718,6 +1727,9 @@
                 </c:pt>
                 <c:pt idx="115">
                   <c:v>3255</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>3238</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2115,6 +2127,9 @@
                 <c:pt idx="115">
                   <c:v>44904</c:v>
                 </c:pt>
+                <c:pt idx="116">
+                  <c:v>44908</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2471,6 +2486,9 @@
                 </c:pt>
                 <c:pt idx="115">
                   <c:v>434</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>436</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2899,6 +2917,9 @@
                 <c:pt idx="115">
                   <c:v>44904</c:v>
                 </c:pt>
+                <c:pt idx="116">
+                  <c:v>44908</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3255,6 +3276,9 @@
                 </c:pt>
                 <c:pt idx="115">
                   <c:v>381</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>380</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4482,13 +4506,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K118"/>
+  <dimension ref="A1:K119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I119" sqref="I119"/>
+      <selection pane="bottomRight" activeCell="I120" sqref="I120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8876,6 +8900,43 @@
       </c>
       <c r="K118" s="7">
         <v>381</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
+        <v>44908</v>
+      </c>
+      <c r="B119" s="2">
+        <v>9</v>
+      </c>
+      <c r="C119">
+        <f t="shared" ref="C119" si="155">SUM(D119:F119)</f>
+        <v>1673</v>
+      </c>
+      <c r="D119">
+        <v>1105</v>
+      </c>
+      <c r="E119">
+        <v>371</v>
+      </c>
+      <c r="F119" s="3">
+        <v>197</v>
+      </c>
+      <c r="G119" s="4">
+        <v>39</v>
+      </c>
+      <c r="H119">
+        <f t="shared" ref="H119" si="156">SUM(I119:K119)</f>
+        <v>4054</v>
+      </c>
+      <c r="I119" s="5">
+        <v>3238</v>
+      </c>
+      <c r="J119" s="6">
+        <v>436</v>
+      </c>
+      <c r="K119" s="7">
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Linecount update (for NavigationStack branch)
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A541561B-1D5B-3646-B736-248931D4D951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5E610B-0D61-364A-8099-50E016C0FB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -614,6 +614,9 @@
                 <c:pt idx="116">
                   <c:v>44908</c:v>
                 </c:pt>
+                <c:pt idx="117">
+                  <c:v>44910</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -973,6 +976,9 @@
                 </c:pt>
                 <c:pt idx="116">
                   <c:v>4054</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>4061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1371,6 +1377,9 @@
                 <c:pt idx="116">
                   <c:v>44908</c:v>
                 </c:pt>
+                <c:pt idx="117">
+                  <c:v>44910</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1730,6 +1739,9 @@
                 </c:pt>
                 <c:pt idx="116">
                   <c:v>3238</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>3244</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2130,6 +2142,9 @@
                 <c:pt idx="116">
                   <c:v>44908</c:v>
                 </c:pt>
+                <c:pt idx="117">
+                  <c:v>44910</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2488,6 +2503,9 @@
                   <c:v>434</c:v>
                 </c:pt>
                 <c:pt idx="116">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="117">
                   <c:v>436</c:v>
                 </c:pt>
               </c:numCache>
@@ -2920,6 +2938,9 @@
                 <c:pt idx="116">
                   <c:v>44908</c:v>
                 </c:pt>
+                <c:pt idx="117">
+                  <c:v>44910</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3279,6 +3300,9 @@
                 </c:pt>
                 <c:pt idx="116">
                   <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>381</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4210,7 +4234,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4498,7 +4522,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4506,13 +4530,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K119"/>
+  <dimension ref="A1:K120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I120" sqref="I120"/>
+      <selection pane="bottomRight" activeCell="I121" sqref="I121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8937,6 +8961,43 @@
       </c>
       <c r="K119" s="7">
         <v>380</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
+        <v>44910</v>
+      </c>
+      <c r="B120" s="2">
+        <v>9</v>
+      </c>
+      <c r="C120">
+        <f t="shared" ref="C120" si="157">SUM(D120:F120)</f>
+        <v>1673</v>
+      </c>
+      <c r="D120">
+        <v>1105</v>
+      </c>
+      <c r="E120">
+        <v>371</v>
+      </c>
+      <c r="F120" s="3">
+        <v>197</v>
+      </c>
+      <c r="G120" s="4">
+        <v>39</v>
+      </c>
+      <c r="H120">
+        <f t="shared" ref="H120" si="158">SUM(I120:K120)</f>
+        <v>4061</v>
+      </c>
+      <c r="I120" s="5">
+        <v>3244</v>
+      </c>
+      <c r="J120" s="6">
+        <v>436</v>
+      </c>
+      <c r="K120" s="7">
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: #80 renamed AnimatedLogoView to PreludeView
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650F3287-73C7-C143-9EDF-9454BD4FACBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B734FA83-446C-5A4E-8D71-F38498F41855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -629,6 +629,9 @@
                 <c:pt idx="121">
                   <c:v>44916</c:v>
                 </c:pt>
+                <c:pt idx="122">
+                  <c:v>44917</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1003,6 +1006,9 @@
                 </c:pt>
                 <c:pt idx="121">
                   <c:v>4092</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>4100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1416,6 +1422,9 @@
                 <c:pt idx="121">
                   <c:v>44916</c:v>
                 </c:pt>
+                <c:pt idx="122">
+                  <c:v>44917</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1790,6 +1799,9 @@
                 </c:pt>
                 <c:pt idx="121">
                   <c:v>3275</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>3281</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2205,6 +2217,9 @@
                 <c:pt idx="121">
                   <c:v>44916</c:v>
                 </c:pt>
+                <c:pt idx="122">
+                  <c:v>44917</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2578,6 +2593,9 @@
                   <c:v>435</c:v>
                 </c:pt>
                 <c:pt idx="121">
+                  <c:v>434</c:v>
+                </c:pt>
+                <c:pt idx="122">
                   <c:v>434</c:v>
                 </c:pt>
               </c:numCache>
@@ -3025,6 +3043,9 @@
                 <c:pt idx="121">
                   <c:v>44916</c:v>
                 </c:pt>
+                <c:pt idx="122">
+                  <c:v>44917</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3399,6 +3420,9 @@
                 </c:pt>
                 <c:pt idx="121">
                   <c:v>383</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>385</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4626,13 +4650,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K124"/>
+  <dimension ref="A1:K125"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A124" sqref="A124:XFD124"/>
+      <selection pane="bottomRight" activeCell="P118" sqref="P118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9117,7 +9141,7 @@
         <v>197</v>
       </c>
       <c r="G121" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H121">
         <f t="shared" ref="H121" si="160">SUM(I121:K121)</f>
@@ -9154,7 +9178,7 @@
         <v>197</v>
       </c>
       <c r="G122" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H122">
         <f t="shared" ref="H122" si="162">SUM(I122:K122)</f>
@@ -9191,7 +9215,7 @@
         <v>197</v>
       </c>
       <c r="G123" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H123">
         <f t="shared" ref="H123" si="164">SUM(I123:K123)</f>
@@ -9228,7 +9252,7 @@
         <v>197</v>
       </c>
       <c r="G124" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H124">
         <f t="shared" ref="H124" si="166">SUM(I124:K124)</f>
@@ -9242,6 +9266,43 @@
       </c>
       <c r="K124" s="7">
         <v>383</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
+        <v>44917</v>
+      </c>
+      <c r="B125" s="2">
+        <v>9</v>
+      </c>
+      <c r="C125">
+        <f t="shared" ref="C125" si="167">SUM(D125:F125)</f>
+        <v>1673</v>
+      </c>
+      <c r="D125">
+        <v>1105</v>
+      </c>
+      <c r="E125">
+        <v>371</v>
+      </c>
+      <c r="F125" s="3">
+        <v>197</v>
+      </c>
+      <c r="G125" s="4">
+        <v>40</v>
+      </c>
+      <c r="H125">
+        <f t="shared" ref="H125" si="168">SUM(I125:K125)</f>
+        <v>4100</v>
+      </c>
+      <c r="I125" s="5">
+        <v>3281</v>
+      </c>
+      <c r="J125" s="6">
+        <v>434</v>
+      </c>
+      <c r="K125" s="7">
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -9261,7 +9322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA41" sqref="AA41"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated stripOffTagsFromName to Swift 5.7 Regex
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF02296-DB8F-A044-87EA-373F15D29FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875CEB27-6C9B-8A47-ACDA-95C170DFB69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -638,6 +638,9 @@
                 <c:pt idx="124">
                   <c:v>44919</c:v>
                 </c:pt>
+                <c:pt idx="125">
+                  <c:v>44919</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1021,6 +1024,9 @@
                 </c:pt>
                 <c:pt idx="124">
                   <c:v>4192</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>4240</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1443,6 +1449,9 @@
                 <c:pt idx="124">
                   <c:v>44919</c:v>
                 </c:pt>
+                <c:pt idx="125">
+                  <c:v>44919</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1826,6 +1835,9 @@
                 </c:pt>
                 <c:pt idx="124">
                   <c:v>3339</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>3379</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2250,6 +2262,9 @@
                 <c:pt idx="124">
                   <c:v>44919</c:v>
                 </c:pt>
+                <c:pt idx="125">
+                  <c:v>44919</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2633,6 +2648,9 @@
                 </c:pt>
                 <c:pt idx="124">
                   <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>461</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3088,6 +3106,9 @@
                 <c:pt idx="124">
                   <c:v>44919</c:v>
                 </c:pt>
+                <c:pt idx="125">
+                  <c:v>44919</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3471,6 +3492,9 @@
                 </c:pt>
                 <c:pt idx="124">
                   <c:v>398</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4698,13 +4722,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K127"/>
+  <dimension ref="A1:K128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I128" sqref="I128"/>
+      <selection pane="bottomRight" activeCell="I129" sqref="I129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9425,6 +9449,43 @@
       </c>
       <c r="K127" s="7">
         <v>398</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
+        <v>44919</v>
+      </c>
+      <c r="B128" s="2">
+        <v>9</v>
+      </c>
+      <c r="C128">
+        <f t="shared" ref="C128" si="173">SUM(D128:F128)</f>
+        <v>1673</v>
+      </c>
+      <c r="D128">
+        <v>1105</v>
+      </c>
+      <c r="E128">
+        <v>371</v>
+      </c>
+      <c r="F128" s="3">
+        <v>197</v>
+      </c>
+      <c r="G128" s="4">
+        <v>43</v>
+      </c>
+      <c r="H128">
+        <f t="shared" ref="H128" si="174">SUM(I128:K128)</f>
+        <v>4240</v>
+      </c>
+      <c r="I128" s="5">
+        <v>3379</v>
+      </c>
+      <c r="J128" s="6">
+        <v>461</v>
+      </c>
+      <c r="K128" s="7">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved string extraction from FGWMembersProvider into separate source files.
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875CEB27-6C9B-8A47-ACDA-95C170DFB69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278FB2D4-98C0-3743-A0D7-D35E83CBEF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1026,7 +1026,7 @@
                   <c:v>4192</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>4240</c:v>
+                  <c:v>4296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1837,7 +1837,7 @@
                   <c:v>3339</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>3379</c:v>
+                  <c:v>3410</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2650,7 +2650,7 @@
                   <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>461</c:v>
+                  <c:v>475</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3494,7 +3494,7 @@
                   <c:v>398</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>400</c:v>
+                  <c:v>411</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9476,16 +9476,16 @@
       </c>
       <c r="H128">
         <f t="shared" ref="H128" si="174">SUM(I128:K128)</f>
-        <v>4240</v>
+        <v>4296</v>
       </c>
       <c r="I128" s="5">
-        <v>3379</v>
+        <v>3410</v>
       </c>
       <c r="J128" s="6">
-        <v>461</v>
+        <v>475</v>
       </c>
       <c r="K128" s="7">
-        <v>400</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Convert componentizePersonName() to user Swift 5.7 RegEx
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D508A8-A84C-7447-A9AD-D243213FD117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8856CB-2AD0-9542-840F-B59D6F4B081B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1032,7 +1032,7 @@
                   <c:v>4296</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>4379</c:v>
+                  <c:v>4420</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1849,7 +1849,7 @@
                   <c:v>3410</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>3448</c:v>
+                  <c:v>3484</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2668,7 +2668,7 @@
                   <c:v>475</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>501</c:v>
+                  <c:v>504</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3518,7 +3518,7 @@
                   <c:v>411</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>430</c:v>
+                  <c:v>432</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9537,16 +9537,16 @@
       </c>
       <c r="H129">
         <f t="shared" ref="H129" si="176">SUM(I129:K129)</f>
-        <v>4379</v>
+        <v>4420</v>
       </c>
       <c r="I129" s="5">
-        <v>3448</v>
+        <v>3484</v>
       </c>
       <c r="J129" s="6">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="K129" s="7">
-        <v>430</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix #88 Removed old Regex extension to String (now that all code uses Swift 5.7 Regex support)
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8856CB-2AD0-9542-840F-B59D6F4B081B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1189971C-2016-6541-93FB-5F483C040187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -1032,7 +1032,7 @@
                   <c:v>4296</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>4420</c:v>
+                  <c:v>4414</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1849,7 +1849,7 @@
                   <c:v>3410</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>3484</c:v>
+                  <c:v>3464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2668,7 +2668,7 @@
                   <c:v>475</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>504</c:v>
+                  <c:v>518</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4752,7 +4752,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I130" sqref="I130"/>
+      <selection pane="bottomRight" activeCell="G129" sqref="G129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9533,17 +9533,17 @@
         <v>197</v>
       </c>
       <c r="G129" s="4">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="H129">
         <f t="shared" ref="H129" si="176">SUM(I129:K129)</f>
-        <v>4420</v>
+        <v>4414</v>
       </c>
       <c r="I129" s="5">
-        <v>3484</v>
+        <v>3464</v>
       </c>
       <c r="J129" s="6">
-        <v>504</v>
+        <v>518</v>
       </c>
       <c r="K129" s="7">
         <v>432</v>

</xml_diff>

<commit_message>
Cleaned up logging. Including make more explicit which photo club is involved.
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1189971C-2016-6541-93FB-5F483C040187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2F105C-4FEC-9343-B776-5A5670A656D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -644,6 +644,9 @@
                 <c:pt idx="126">
                   <c:v>44922</c:v>
                 </c:pt>
+                <c:pt idx="127">
+                  <c:v>44923</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1033,6 +1036,9 @@
                 </c:pt>
                 <c:pt idx="126">
                   <c:v>4414</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>4386</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1461,6 +1467,9 @@
                 <c:pt idx="126">
                   <c:v>44922</c:v>
                 </c:pt>
+                <c:pt idx="127">
+                  <c:v>44923</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1850,6 +1859,9 @@
                 </c:pt>
                 <c:pt idx="126">
                   <c:v>3464</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>3455</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2280,6 +2292,9 @@
                 <c:pt idx="126">
                   <c:v>44922</c:v>
                 </c:pt>
+                <c:pt idx="127">
+                  <c:v>44923</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2669,6 +2684,9 @@
                 </c:pt>
                 <c:pt idx="126">
                   <c:v>518</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>514</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3130,6 +3148,9 @@
                 <c:pt idx="126">
                   <c:v>44922</c:v>
                 </c:pt>
+                <c:pt idx="127">
+                  <c:v>44923</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3519,6 +3540,9 @@
                 </c:pt>
                 <c:pt idx="126">
                   <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>417</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4746,13 +4770,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K129"/>
+  <dimension ref="A1:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G129" sqref="G129"/>
+      <selection pane="bottomRight" activeCell="I131" sqref="I131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9547,6 +9571,43 @@
       </c>
       <c r="K129" s="7">
         <v>432</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
+        <v>44923</v>
+      </c>
+      <c r="B130" s="2">
+        <v>9</v>
+      </c>
+      <c r="C130">
+        <f t="shared" ref="C130" si="177">SUM(D130:F130)</f>
+        <v>1673</v>
+      </c>
+      <c r="D130">
+        <v>1105</v>
+      </c>
+      <c r="E130">
+        <v>371</v>
+      </c>
+      <c r="F130" s="3">
+        <v>197</v>
+      </c>
+      <c r="G130" s="4">
+        <v>50</v>
+      </c>
+      <c r="H130">
+        <f t="shared" ref="H130" si="178">SUM(I130:K130)</f>
+        <v>4386</v>
+      </c>
+      <c r="I130" s="5">
+        <v>3455</v>
+      </c>
+      <c r="J130" s="6">
+        <v>514</v>
+      </c>
+      <c r="K130" s="7">
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -9566,8 +9627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA41" sqref="AA41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA35" sqref="AA35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix: #112 large tuple warning, so PhotoClubID is now a struct with 3 fields.
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC384C2-F51C-3843-88DE-FDF13A480223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7642399-0E13-0648-8130-517712134A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -653,6 +653,9 @@
                 <c:pt idx="129">
                   <c:v>44930</c:v>
                 </c:pt>
+                <c:pt idx="130">
+                  <c:v>44936</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1051,6 +1054,9 @@
                 </c:pt>
                 <c:pt idx="129">
                   <c:v>4350</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>4367</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1488,6 +1494,9 @@
                 <c:pt idx="129">
                   <c:v>44930</c:v>
                 </c:pt>
+                <c:pt idx="130">
+                  <c:v>44936</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1886,6 +1895,9 @@
                 </c:pt>
                 <c:pt idx="129">
                   <c:v>3449</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>3457</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2325,6 +2337,9 @@
                 <c:pt idx="129">
                   <c:v>44930</c:v>
                 </c:pt>
+                <c:pt idx="130">
+                  <c:v>44936</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2723,6 +2738,9 @@
                 </c:pt>
                 <c:pt idx="129">
                   <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3193,6 +3211,9 @@
                 <c:pt idx="129">
                   <c:v>44930</c:v>
                 </c:pt>
+                <c:pt idx="130">
+                  <c:v>44936</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3591,6 +3612,9 @@
                 </c:pt>
                 <c:pt idx="129">
                   <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>418</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4522,7 +4546,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4810,7 +4834,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4818,13 +4842,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K132"/>
+  <dimension ref="A1:K133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I133" sqref="I133"/>
+      <selection pane="bottomRight" activeCell="I134" sqref="I134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9730,6 +9754,43 @@
       </c>
       <c r="K132" s="7">
         <v>415</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <v>44936</v>
+      </c>
+      <c r="B133" s="2">
+        <v>9</v>
+      </c>
+      <c r="C133">
+        <f t="shared" ref="C133" si="183">SUM(D133:F133)</f>
+        <v>1673</v>
+      </c>
+      <c r="D133">
+        <v>1105</v>
+      </c>
+      <c r="E133">
+        <v>371</v>
+      </c>
+      <c r="F133" s="3">
+        <v>197</v>
+      </c>
+      <c r="G133" s="4">
+        <v>51</v>
+      </c>
+      <c r="H133">
+        <f t="shared" ref="H133" si="184">SUM(I133:K133)</f>
+        <v>4367</v>
+      </c>
+      <c r="I133" s="5">
+        <v>3457</v>
+      </c>
+      <c r="J133" s="6">
+        <v>492</v>
+      </c>
+      <c r="K133" s="7">
+        <v>418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: #114 photo club that adds hardcoded member data can not have photographerWebsite data for members
Pretty small change.
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7642399-0E13-0648-8130-517712134A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE70207B-4E8F-4048-8E02-AF75CBA3E51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -656,6 +656,9 @@
                 <c:pt idx="130">
                   <c:v>44936</c:v>
                 </c:pt>
+                <c:pt idx="131">
+                  <c:v>44937</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1057,6 +1060,9 @@
                 </c:pt>
                 <c:pt idx="130">
                   <c:v>4367</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>4370</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1497,6 +1503,9 @@
                 <c:pt idx="130">
                   <c:v>44936</c:v>
                 </c:pt>
+                <c:pt idx="131">
+                  <c:v>44937</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1898,6 +1907,9 @@
                 </c:pt>
                 <c:pt idx="130">
                   <c:v>3457</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>3460</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2340,6 +2352,9 @@
                 <c:pt idx="130">
                   <c:v>44936</c:v>
                 </c:pt>
+                <c:pt idx="131">
+                  <c:v>44937</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2740,6 +2755,9 @@
                   <c:v>486</c:v>
                 </c:pt>
                 <c:pt idx="130">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="131">
                   <c:v>492</c:v>
                 </c:pt>
               </c:numCache>
@@ -3214,6 +3232,9 @@
                 <c:pt idx="130">
                   <c:v>44936</c:v>
                 </c:pt>
+                <c:pt idx="131">
+                  <c:v>44937</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3614,6 +3635,9 @@
                   <c:v>415</c:v>
                 </c:pt>
                 <c:pt idx="130">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="131">
                   <c:v>418</c:v>
                 </c:pt>
               </c:numCache>
@@ -4842,13 +4866,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K133"/>
+  <dimension ref="A1:K134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I134" sqref="I134"/>
+      <selection pane="bottomRight" activeCell="I135" sqref="I135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9790,6 +9814,43 @@
         <v>492</v>
       </c>
       <c r="K133" s="7">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <v>44937</v>
+      </c>
+      <c r="B134" s="2">
+        <v>9</v>
+      </c>
+      <c r="C134">
+        <f t="shared" ref="C134" si="185">SUM(D134:F134)</f>
+        <v>1673</v>
+      </c>
+      <c r="D134">
+        <v>1105</v>
+      </c>
+      <c r="E134">
+        <v>371</v>
+      </c>
+      <c r="F134" s="3">
+        <v>197</v>
+      </c>
+      <c r="G134" s="4">
+        <v>51</v>
+      </c>
+      <c r="H134">
+        <f t="shared" ref="H134" si="186">SUM(I134:K134)</f>
+        <v>4370</v>
+      </c>
+      <c r="I134" s="5">
+        <v>3460</v>
+      </c>
+      <c r="J134" s="6">
+        <v>492</v>
+      </c>
+      <c r="K134" s="7">
         <v>418</v>
       </c>
     </row>
@@ -9811,7 +9872,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA14" sqref="AA14"/>
+      <selection activeCell="AA35" sqref="AA35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated officers of photo club Waalre
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333137DA-B905-824B-9E7A-F6795DE4F25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8400896-FCE0-7845-8182-DD5E4CCB804E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -662,6 +662,9 @@
                 <c:pt idx="132">
                   <c:v>44938</c:v>
                 </c:pt>
+                <c:pt idx="133">
+                  <c:v>44944</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1069,6 +1072,9 @@
                 </c:pt>
                 <c:pt idx="132">
                   <c:v>4446</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>4459</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1515,6 +1521,9 @@
                 <c:pt idx="132">
                   <c:v>44938</c:v>
                 </c:pt>
+                <c:pt idx="133">
+                  <c:v>44944</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1922,6 +1931,9 @@
                 </c:pt>
                 <c:pt idx="132">
                   <c:v>3504</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>3512</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2370,6 +2382,9 @@
                 <c:pt idx="132">
                   <c:v>44938</c:v>
                 </c:pt>
+                <c:pt idx="133">
+                  <c:v>44944</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2777,6 +2792,9 @@
                 </c:pt>
                 <c:pt idx="132">
                   <c:v>508</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>509</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3256,6 +3274,9 @@
                 <c:pt idx="132">
                   <c:v>44938</c:v>
                 </c:pt>
+                <c:pt idx="133">
+                  <c:v>44944</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3663,6 +3684,9 @@
                 </c:pt>
                 <c:pt idx="132">
                   <c:v>434</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>438</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4890,13 +4914,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K135"/>
+  <dimension ref="A1:K136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I136" sqref="I136"/>
+      <selection pane="bottomRight" activeCell="I137" sqref="I137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9913,6 +9937,43 @@
       </c>
       <c r="K135" s="7">
         <v>434</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A136" s="1">
+        <v>44944</v>
+      </c>
+      <c r="B136" s="2">
+        <v>9</v>
+      </c>
+      <c r="C136">
+        <f t="shared" ref="C136" si="189">SUM(D136:F136)</f>
+        <v>1673</v>
+      </c>
+      <c r="D136">
+        <v>1105</v>
+      </c>
+      <c r="E136">
+        <v>371</v>
+      </c>
+      <c r="F136" s="3">
+        <v>197</v>
+      </c>
+      <c r="G136" s="4">
+        <v>51</v>
+      </c>
+      <c r="H136">
+        <f t="shared" ref="H136" si="190">SUM(I136:K136)</f>
+        <v>4459</v>
+      </c>
+      <c r="I136" s="5">
+        <v>3512</v>
+      </c>
+      <c r="J136" s="6">
+        <v>509</v>
+      </c>
+      <c r="K136" s="7">
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -9932,7 +9993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ScrollLock[] lookup now uses PhotoClub.id instead of PhotoClub.fullName
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670C9439-D4CE-3C41-BF54-C1434D4CC6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957291B9-DDBC-A84F-935C-AA6797696D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -668,6 +668,9 @@
                 <c:pt idx="134">
                   <c:v>44947</c:v>
                 </c:pt>
+                <c:pt idx="135">
+                  <c:v>44948</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1081,6 +1084,9 @@
                 </c:pt>
                 <c:pt idx="134">
                   <c:v>4464</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>4493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1533,6 +1539,9 @@
                 <c:pt idx="134">
                   <c:v>44947</c:v>
                 </c:pt>
+                <c:pt idx="135">
+                  <c:v>44948</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1946,6 +1955,9 @@
                 </c:pt>
                 <c:pt idx="134">
                   <c:v>3515</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>3539</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2400,6 +2412,9 @@
                 <c:pt idx="134">
                   <c:v>44947</c:v>
                 </c:pt>
+                <c:pt idx="135">
+                  <c:v>44948</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2812,6 +2827,9 @@
                   <c:v>509</c:v>
                 </c:pt>
                 <c:pt idx="134">
+                  <c:v>511</c:v>
+                </c:pt>
+                <c:pt idx="135">
                   <c:v>511</c:v>
                 </c:pt>
               </c:numCache>
@@ -3298,6 +3316,9 @@
                 <c:pt idx="134">
                   <c:v>44947</c:v>
                 </c:pt>
+                <c:pt idx="135">
+                  <c:v>44948</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3711,6 +3732,9 @@
                 </c:pt>
                 <c:pt idx="134">
                   <c:v>438</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>443</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3803,7 +3827,7 @@
         <c:axId val="1582338719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="4500"/>
+          <c:max val="5000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4938,13 +4962,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K137"/>
+  <dimension ref="A1:K138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I138" sqref="I138"/>
+      <selection pane="bottomRight" activeCell="I139" sqref="I139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10035,6 +10059,43 @@
       </c>
       <c r="K137" s="7">
         <v>438</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A138" s="1">
+        <v>44948</v>
+      </c>
+      <c r="B138" s="2">
+        <v>9</v>
+      </c>
+      <c r="C138">
+        <f t="shared" ref="C138" si="193">SUM(D138:F138)</f>
+        <v>1673</v>
+      </c>
+      <c r="D138">
+        <v>1105</v>
+      </c>
+      <c r="E138">
+        <v>371</v>
+      </c>
+      <c r="F138" s="3">
+        <v>197</v>
+      </c>
+      <c r="G138" s="4">
+        <v>51</v>
+      </c>
+      <c r="H138">
+        <f t="shared" ref="H138" si="194">SUM(I138:K138)</f>
+        <v>4493</v>
+      </c>
+      <c r="I138" s="5">
+        <v>3539</v>
+      </c>
+      <c r="J138" s="6">
+        <v>511</v>
+      </c>
+      <c r="K138" s="7">
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -10054,8 +10115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Renamed Views, added counts to top of Portfolios and Photo Clubs views.
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B26D86-5044-514D-A1CD-C4148348B418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56244D07-DDD5-E741-82B3-DF562D6E77C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -680,6 +680,9 @@
                 <c:pt idx="138">
                   <c:v>44954</c:v>
                 </c:pt>
+                <c:pt idx="139">
+                  <c:v>44962</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1105,6 +1108,9 @@
                 </c:pt>
                 <c:pt idx="138">
                   <c:v>4521</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>4640</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1569,6 +1575,9 @@
                 <c:pt idx="138">
                   <c:v>44954</c:v>
                 </c:pt>
+                <c:pt idx="139">
+                  <c:v>44962</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1994,6 +2003,9 @@
                 </c:pt>
                 <c:pt idx="138">
                   <c:v>3564</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>3646</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2460,6 +2472,9 @@
                 <c:pt idx="138">
                   <c:v>44954</c:v>
                 </c:pt>
+                <c:pt idx="139">
+                  <c:v>44962</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2885,6 +2900,9 @@
                 </c:pt>
                 <c:pt idx="138">
                   <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>526</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3382,6 +3400,9 @@
                 <c:pt idx="138">
                   <c:v>44954</c:v>
                 </c:pt>
+                <c:pt idx="139">
+                  <c:v>44962</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3807,6 +3828,9 @@
                 </c:pt>
                 <c:pt idx="138">
                   <c:v>447</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>468</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3833,8 +3857,8 @@
         <c:axId val="1582352671"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="44960"/>
-          <c:min val="44349"/>
+          <c:max val="44990"/>
+          <c:min val="44379"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -5034,13 +5058,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K141"/>
+  <dimension ref="A1:K142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I142" sqref="I142"/>
+      <selection pane="bottomRight" activeCell="I143" sqref="I143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10279,6 +10303,43 @@
       </c>
       <c r="K141" s="7">
         <v>447</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A142" s="1">
+        <v>44962</v>
+      </c>
+      <c r="B142" s="2">
+        <v>9</v>
+      </c>
+      <c r="C142">
+        <f t="shared" ref="C142" si="201">SUM(D142:F142)</f>
+        <v>1673</v>
+      </c>
+      <c r="D142">
+        <v>1105</v>
+      </c>
+      <c r="E142">
+        <v>371</v>
+      </c>
+      <c r="F142" s="3">
+        <v>197</v>
+      </c>
+      <c r="G142" s="4">
+        <v>51</v>
+      </c>
+      <c r="H142">
+        <f t="shared" ref="H142" si="202">SUM(I142:K142)</f>
+        <v>4640</v>
+      </c>
+      <c r="I142" s="5">
+        <v>3646</v>
+      </c>
+      <c r="J142" s="6">
+        <v>526</v>
+      </c>
+      <c r="K142" s="7">
+        <v>468</v>
       </c>
     </row>
   </sheetData>
@@ -10298,7 +10359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix: #128 Added a count of the photographers in the Who's Who screen
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56244D07-DDD5-E741-82B3-DF562D6E77C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1DD8A2-7F40-624A-B13C-540AE330684A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -683,6 +683,9 @@
                 <c:pt idx="139">
                   <c:v>44962</c:v>
                 </c:pt>
+                <c:pt idx="140">
+                  <c:v>44965</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1111,6 +1114,9 @@
                 </c:pt>
                 <c:pt idx="139">
                   <c:v>4640</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>4651</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1578,6 +1584,9 @@
                 <c:pt idx="139">
                   <c:v>44962</c:v>
                 </c:pt>
+                <c:pt idx="140">
+                  <c:v>44965</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2006,6 +2015,9 @@
                 </c:pt>
                 <c:pt idx="139">
                   <c:v>3646</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>3656</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2475,6 +2487,9 @@
                 <c:pt idx="139">
                   <c:v>44962</c:v>
                 </c:pt>
+                <c:pt idx="140">
+                  <c:v>44965</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2903,6 +2918,9 @@
                 </c:pt>
                 <c:pt idx="139">
                   <c:v>526</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>527</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3403,6 +3421,9 @@
                 <c:pt idx="139">
                   <c:v>44962</c:v>
                 </c:pt>
+                <c:pt idx="140">
+                  <c:v>44965</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3830,6 +3851,9 @@
                   <c:v>447</c:v>
                 </c:pt>
                 <c:pt idx="139">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="140">
                   <c:v>468</c:v>
                 </c:pt>
               </c:numCache>
@@ -5058,13 +5082,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K142"/>
+  <dimension ref="A1:K143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I143" sqref="I143"/>
+      <selection pane="bottomRight" activeCell="I144" sqref="I144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10339,6 +10363,43 @@
         <v>526</v>
       </c>
       <c r="K142" s="7">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A143" s="1">
+        <v>44965</v>
+      </c>
+      <c r="B143" s="2">
+        <v>9</v>
+      </c>
+      <c r="C143">
+        <f t="shared" ref="C143" si="203">SUM(D143:F143)</f>
+        <v>1673</v>
+      </c>
+      <c r="D143">
+        <v>1105</v>
+      </c>
+      <c r="E143">
+        <v>371</v>
+      </c>
+      <c r="F143" s="3">
+        <v>197</v>
+      </c>
+      <c r="G143" s="4">
+        <v>51</v>
+      </c>
+      <c r="H143">
+        <f t="shared" ref="H143" si="204">SUM(I143:K143)</f>
+        <v>4651</v>
+      </c>
+      <c r="I143" s="5">
+        <v>3656</v>
+      </c>
+      <c r="J143" s="6">
+        <v>527</v>
+      </c>
+      <c r="K143" s="7">
         <v>468</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sections (with headers and footers) in MemberPortfolio screen
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1DD8A2-7F40-624A-B13C-540AE330684A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22934EF-1BAA-4845-9556-999069DD46F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -686,6 +686,9 @@
                 <c:pt idx="140">
                   <c:v>44965</c:v>
                 </c:pt>
+                <c:pt idx="141">
+                  <c:v>44968</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1117,6 +1120,9 @@
                 </c:pt>
                 <c:pt idx="140">
                   <c:v>4651</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>4696</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1587,6 +1593,9 @@
                 <c:pt idx="140">
                   <c:v>44965</c:v>
                 </c:pt>
+                <c:pt idx="141">
+                  <c:v>44968</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2018,6 +2027,9 @@
                 </c:pt>
                 <c:pt idx="140">
                   <c:v>3656</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>3697</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2490,6 +2502,9 @@
                 <c:pt idx="140">
                   <c:v>44965</c:v>
                 </c:pt>
+                <c:pt idx="141">
+                  <c:v>44968</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2921,6 +2936,9 @@
                 </c:pt>
                 <c:pt idx="140">
                   <c:v>527</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>529</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3424,6 +3442,9 @@
                 <c:pt idx="140">
                   <c:v>44965</c:v>
                 </c:pt>
+                <c:pt idx="141">
+                  <c:v>44968</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3855,6 +3876,9 @@
                 </c:pt>
                 <c:pt idx="140">
                   <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>470</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5082,13 +5106,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K143"/>
+  <dimension ref="A1:K144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I144" sqref="I144"/>
+      <selection pane="bottomRight" activeCell="I145" sqref="I145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10401,6 +10425,43 @@
       </c>
       <c r="K143" s="7">
         <v>468</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <v>44968</v>
+      </c>
+      <c r="B144" s="2">
+        <v>9</v>
+      </c>
+      <c r="C144">
+        <f t="shared" ref="C144" si="205">SUM(D144:F144)</f>
+        <v>1673</v>
+      </c>
+      <c r="D144">
+        <v>1105</v>
+      </c>
+      <c r="E144">
+        <v>371</v>
+      </c>
+      <c r="F144" s="3">
+        <v>197</v>
+      </c>
+      <c r="G144" s="4">
+        <v>51</v>
+      </c>
+      <c r="H144">
+        <f t="shared" ref="H144" si="206">SUM(I144:K144)</f>
+        <v>4696</v>
+      </c>
+      <c r="I144" s="5">
+        <v>3697</v>
+      </c>
+      <c r="J144" s="6">
+        <v>529</v>
+      </c>
+      <c r="K144" s="7">
+        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: #134 Get searchbar working with sectionedFetchRequest
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22934EF-1BAA-4845-9556-999069DD46F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9A96C4-D039-2741-8359-10DE8B049291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -689,6 +689,9 @@
                 <c:pt idx="141">
                   <c:v>44968</c:v>
                 </c:pt>
+                <c:pt idx="142">
+                  <c:v>44971</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1123,6 +1126,9 @@
                 </c:pt>
                 <c:pt idx="141">
                   <c:v>4696</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>4699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1596,6 +1602,9 @@
                 <c:pt idx="141">
                   <c:v>44968</c:v>
                 </c:pt>
+                <c:pt idx="142">
+                  <c:v>44971</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2030,6 +2039,9 @@
                 </c:pt>
                 <c:pt idx="141">
                   <c:v>3697</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>3700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2505,6 +2517,9 @@
                 <c:pt idx="141">
                   <c:v>44968</c:v>
                 </c:pt>
+                <c:pt idx="142">
+                  <c:v>44971</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2938,6 +2953,9 @@
                   <c:v>527</c:v>
                 </c:pt>
                 <c:pt idx="141">
+                  <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="142">
                   <c:v>529</c:v>
                 </c:pt>
               </c:numCache>
@@ -3445,6 +3463,9 @@
                 <c:pt idx="141">
                   <c:v>44968</c:v>
                 </c:pt>
+                <c:pt idx="142">
+                  <c:v>44971</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3878,6 +3899,9 @@
                   <c:v>468</c:v>
                 </c:pt>
                 <c:pt idx="141">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="142">
                   <c:v>470</c:v>
                 </c:pt>
               </c:numCache>
@@ -5106,13 +5130,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K144"/>
+  <dimension ref="A1:K145"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I145" sqref="I145"/>
+      <selection pane="bottomRight" activeCell="I146" sqref="I146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10461,6 +10485,43 @@
         <v>529</v>
       </c>
       <c r="K144" s="7">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <v>44971</v>
+      </c>
+      <c r="B145" s="2">
+        <v>9</v>
+      </c>
+      <c r="C145">
+        <f t="shared" ref="C145" si="207">SUM(D145:F145)</f>
+        <v>1673</v>
+      </c>
+      <c r="D145">
+        <v>1105</v>
+      </c>
+      <c r="E145">
+        <v>371</v>
+      </c>
+      <c r="F145" s="3">
+        <v>197</v>
+      </c>
+      <c r="G145" s="4">
+        <v>51</v>
+      </c>
+      <c r="H145">
+        <f t="shared" ref="H145" si="208">SUM(I145:K145)</f>
+        <v>4699</v>
+      </c>
+      <c r="I145" s="5">
+        <v>3700</v>
+      </c>
+      <c r="J145" s="6">
+        <v>529</v>
+      </c>
+      <c r="K145" s="7">
         <v>470</v>
       </c>
     </row>
@@ -10481,7 +10542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix: #135. Counts in section footers on Portfolios screen
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9A96C4-D039-2741-8359-10DE8B049291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2226D53-BDCB-DB48-948E-67004ADB739A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
     <sheet name="Graph" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Table!$A$3:$A$149</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Table!$H$3:$H$149</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Table!$I$3:$I$149</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Table!$J$3:$J$149</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Table!$K$3:$K$149</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Table!$A$3:$A$149</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Table!$H$3:$H$149</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Table!$I$3:$I$149</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Table!$J$3:$J$149</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Table!$K$3:$K$149</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -692,6 +704,9 @@
                 <c:pt idx="142">
                   <c:v>44971</c:v>
                 </c:pt>
+                <c:pt idx="143">
+                  <c:v>44972</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1129,6 +1144,9 @@
                 </c:pt>
                 <c:pt idx="142">
                   <c:v>4699</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>4706</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1605,6 +1623,9 @@
                 <c:pt idx="142">
                   <c:v>44971</c:v>
                 </c:pt>
+                <c:pt idx="143">
+                  <c:v>44972</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2042,6 +2063,9 @@
                 </c:pt>
                 <c:pt idx="142">
                   <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>3707</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2520,6 +2544,9 @@
                 <c:pt idx="142">
                   <c:v>44971</c:v>
                 </c:pt>
+                <c:pt idx="143">
+                  <c:v>44972</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2956,6 +2983,9 @@
                   <c:v>529</c:v>
                 </c:pt>
                 <c:pt idx="142">
+                  <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="143">
                   <c:v>529</c:v>
                 </c:pt>
               </c:numCache>
@@ -3001,19 +3031,7 @@
           <c:dPt>
             <c:idx val="61"/>
             <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent4"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
+              <c:symbol val="none"/>
             </c:marker>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -3466,6 +3484,9 @@
                 <c:pt idx="142">
                   <c:v>44971</c:v>
                 </c:pt>
+                <c:pt idx="143">
+                  <c:v>44972</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3902,6 +3923,9 @@
                   <c:v>470</c:v>
                 </c:pt>
                 <c:pt idx="142">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="143">
                   <c:v>470</c:v>
                 </c:pt>
               </c:numCache>
@@ -3948,7 +3972,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="[$]\ mmm\ d\,\ yyyy;@" c16r2:formatcode2="[$-en-NL,1]\ mmm\ d\,\ yyyy;@" sourceLinked="0"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="0"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
@@ -4147,8 +4171,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.6393516697157211"/>
           <c:y val="0.59630513927694528"/>
-          <c:w val="8.6045271289377251E-2"/>
-          <c:h val="0.14401330501945014"/>
+          <c:w val="7.1125922625114371E-2"/>
+          <c:h val="0.1179698432124137"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -5130,13 +5154,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K145"/>
+  <dimension ref="A1:K146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B84" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I146" sqref="I146"/>
+      <selection pane="bottomRight" activeCell="A147" sqref="A147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10522,6 +10546,43 @@
         <v>529</v>
       </c>
       <c r="K145" s="7">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A146" s="1">
+        <v>44972</v>
+      </c>
+      <c r="B146" s="2">
+        <v>9</v>
+      </c>
+      <c r="C146">
+        <f t="shared" ref="C146" si="209">SUM(D146:F146)</f>
+        <v>1673</v>
+      </c>
+      <c r="D146">
+        <v>1105</v>
+      </c>
+      <c r="E146">
+        <v>371</v>
+      </c>
+      <c r="F146" s="3">
+        <v>197</v>
+      </c>
+      <c r="G146" s="4">
+        <v>51</v>
+      </c>
+      <c r="H146">
+        <f t="shared" ref="H146" si="210">SUM(I146:K146)</f>
+        <v>4706</v>
+      </c>
+      <c r="I146" s="5">
+        <v>3707</v>
+      </c>
+      <c r="J146" s="6">
+        <v>529</v>
+      </c>
+      <c r="K146" s="7">
         <v>470</v>
       </c>
     </row>
@@ -10542,7 +10603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix: 138. New SwiftUI file named MemberPortfolioView. Was previously nested inside SinglePortFolioView.
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2226D53-BDCB-DB48-948E-67004ADB739A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C9C59A-8C73-2445-A5C7-53E5F27D483F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -16,18 +16,6 @@
     <sheet name="Table" sheetId="1" r:id="rId1"/>
     <sheet name="Graph" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Table!$A$3:$A$149</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Table!$H$3:$H$149</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Table!$I$3:$I$149</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Table!$J$3:$J$149</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Table!$K$3:$K$149</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Table!$A$3:$A$149</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Table!$H$3:$H$149</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Table!$I$3:$I$149</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Table!$J$3:$J$149</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Table!$K$3:$K$149</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -707,6 +695,9 @@
                 <c:pt idx="143">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="144">
+                  <c:v>44974</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1147,6 +1138,9 @@
                 </c:pt>
                 <c:pt idx="143">
                   <c:v>4706</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>4722</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1626,6 +1620,9 @@
                 <c:pt idx="143">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="144">
+                  <c:v>44974</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2065,6 +2062,9 @@
                   <c:v>3700</c:v>
                 </c:pt>
                 <c:pt idx="143">
+                  <c:v>3707</c:v>
+                </c:pt>
+                <c:pt idx="144">
                   <c:v>3707</c:v>
                 </c:pt>
               </c:numCache>
@@ -2547,6 +2547,9 @@
                 <c:pt idx="143">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="144">
+                  <c:v>44974</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2987,6 +2990,9 @@
                 </c:pt>
                 <c:pt idx="143">
                   <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>540</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3487,6 +3493,9 @@
                 <c:pt idx="143">
                   <c:v>44972</c:v>
                 </c:pt>
+                <c:pt idx="144">
+                  <c:v>44974</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3927,6 +3936,9 @@
                 </c:pt>
                 <c:pt idx="143">
                   <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>475</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5154,13 +5166,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K146"/>
+  <dimension ref="A1:K147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B84" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A147" sqref="A147"/>
+      <selection pane="bottomRight" activeCell="I148" sqref="I148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10584,6 +10596,43 @@
       </c>
       <c r="K146" s="7">
         <v>470</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A147" s="1">
+        <v>44974</v>
+      </c>
+      <c r="B147" s="2">
+        <v>9</v>
+      </c>
+      <c r="C147">
+        <f t="shared" ref="C147" si="211">SUM(D147:F147)</f>
+        <v>1673</v>
+      </c>
+      <c r="D147">
+        <v>1105</v>
+      </c>
+      <c r="E147">
+        <v>371</v>
+      </c>
+      <c r="F147" s="3">
+        <v>197</v>
+      </c>
+      <c r="G147" s="4">
+        <v>52</v>
+      </c>
+      <c r="H147">
+        <f t="shared" ref="H147" si="212">SUM(I147:K147)</f>
+        <v>4722</v>
+      </c>
+      <c r="I147" s="5">
+        <v>3707</v>
+      </c>
+      <c r="J147" s="6">
+        <v>540</v>
+      </c>
+      <c r="K147" s="7">
+        <v>475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Converted Settings to a Bottom Sheet (was a popup)
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB981222-28B7-A54D-B0B9-C5BD043BB908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA9B5CB-48BE-2F46-BE3B-8C02FF627F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -701,6 +701,9 @@
                 <c:pt idx="145">
                   <c:v>44975</c:v>
                 </c:pt>
+                <c:pt idx="146">
+                  <c:v>44976</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1147,6 +1150,9 @@
                 </c:pt>
                 <c:pt idx="145">
                   <c:v>4735</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>4744</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1632,6 +1638,9 @@
                 <c:pt idx="145">
                   <c:v>44975</c:v>
                 </c:pt>
+                <c:pt idx="146">
+                  <c:v>44976</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2078,6 +2087,9 @@
                 </c:pt>
                 <c:pt idx="145">
                   <c:v>3716</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>3724</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2565,6 +2577,9 @@
                 <c:pt idx="145">
                   <c:v>44975</c:v>
                 </c:pt>
+                <c:pt idx="146">
+                  <c:v>44976</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3010,6 +3025,9 @@
                   <c:v>540</c:v>
                 </c:pt>
                 <c:pt idx="145">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="146">
                   <c:v>544</c:v>
                 </c:pt>
               </c:numCache>
@@ -3517,6 +3535,9 @@
                 <c:pt idx="145">
                   <c:v>44975</c:v>
                 </c:pt>
+                <c:pt idx="146">
+                  <c:v>44976</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3963,6 +3984,9 @@
                 </c:pt>
                 <c:pt idx="145">
                   <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>476</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5190,13 +5214,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K148"/>
+  <dimension ref="A1:K150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P101" sqref="P101"/>
+      <selection pane="bottomRight" activeCell="I151" sqref="I151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10694,6 +10718,80 @@
       </c>
       <c r="K148" s="7">
         <v>475</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A149" s="1">
+        <v>44976</v>
+      </c>
+      <c r="B149" s="2">
+        <v>9</v>
+      </c>
+      <c r="C149">
+        <f t="shared" ref="C149" si="215">SUM(D149:F149)</f>
+        <v>1673</v>
+      </c>
+      <c r="D149">
+        <v>1105</v>
+      </c>
+      <c r="E149">
+        <v>371</v>
+      </c>
+      <c r="F149" s="3">
+        <v>197</v>
+      </c>
+      <c r="G149" s="4">
+        <v>52</v>
+      </c>
+      <c r="H149">
+        <f t="shared" ref="H149" si="216">SUM(I149:K149)</f>
+        <v>4744</v>
+      </c>
+      <c r="I149" s="5">
+        <v>3724</v>
+      </c>
+      <c r="J149" s="6">
+        <v>544</v>
+      </c>
+      <c r="K149" s="7">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A150" s="1">
+        <v>44977</v>
+      </c>
+      <c r="B150" s="2">
+        <v>9</v>
+      </c>
+      <c r="C150">
+        <f t="shared" ref="C150" si="217">SUM(D150:F150)</f>
+        <v>1673</v>
+      </c>
+      <c r="D150">
+        <v>1105</v>
+      </c>
+      <c r="E150">
+        <v>371</v>
+      </c>
+      <c r="F150" s="3">
+        <v>197</v>
+      </c>
+      <c r="G150" s="4">
+        <v>52</v>
+      </c>
+      <c r="H150">
+        <f t="shared" ref="H150" si="218">SUM(I150:K150)</f>
+        <v>5767</v>
+      </c>
+      <c r="I150" s="5">
+        <v>4747</v>
+      </c>
+      <c r="J150" s="6">
+        <v>544</v>
+      </c>
+      <c r="K150" s="7">
+        <v>476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: #146 Show data source(s) below each section of the Portfolios screen.
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57933A3F-D29A-1649-9A1A-CC31DAC9CE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E23BDF-21BD-D844-BA4C-FC446F9F10AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26560" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -710,6 +710,9 @@
                 <c:pt idx="148">
                   <c:v>44979</c:v>
                 </c:pt>
+                <c:pt idx="149">
+                  <c:v>44983</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1165,6 +1168,9 @@
                 </c:pt>
                 <c:pt idx="148">
                   <c:v>4747</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>4784</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1659,6 +1665,9 @@
                 <c:pt idx="148">
                   <c:v>44979</c:v>
                 </c:pt>
+                <c:pt idx="149">
+                  <c:v>44983</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2114,6 +2123,9 @@
                 </c:pt>
                 <c:pt idx="148">
                   <c:v>3726</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>3746</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2610,6 +2622,9 @@
                 <c:pt idx="148">
                   <c:v>44979</c:v>
                 </c:pt>
+                <c:pt idx="149">
+                  <c:v>44983</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3065,6 +3080,9 @@
                 </c:pt>
                 <c:pt idx="148">
                   <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>549</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3580,6 +3598,9 @@
                 <c:pt idx="148">
                   <c:v>44979</c:v>
                 </c:pt>
+                <c:pt idx="149">
+                  <c:v>44983</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4035,6 +4056,9 @@
                 </c:pt>
                 <c:pt idx="148">
                   <c:v>477</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>489</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5262,13 +5286,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K151"/>
+  <dimension ref="A1:K152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B99" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I152" sqref="I152"/>
+      <selection pane="bottomRight" activeCell="I153" sqref="I153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10877,6 +10901,43 @@
       </c>
       <c r="K151" s="7">
         <v>477</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A152" s="1">
+        <v>44983</v>
+      </c>
+      <c r="B152" s="2">
+        <v>9</v>
+      </c>
+      <c r="C152">
+        <f t="shared" ref="C152" si="221">SUM(D152:F152)</f>
+        <v>1673</v>
+      </c>
+      <c r="D152">
+        <v>1105</v>
+      </c>
+      <c r="E152">
+        <v>371</v>
+      </c>
+      <c r="F152" s="3">
+        <v>197</v>
+      </c>
+      <c r="G152" s="4">
+        <v>52</v>
+      </c>
+      <c r="H152">
+        <f t="shared" ref="H152" si="222">SUM(I152:K152)</f>
+        <v>4784</v>
+      </c>
+      <c r="I152" s="5">
+        <v>3746</v>
+      </c>
+      <c r="J152" s="6">
+        <v>549</v>
+      </c>
+      <c r="K152" s="7">
+        <v>489</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed color of section header to grey (PortfoliosView.swift)
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E23BDF-21BD-D844-BA4C-FC446F9F10AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA17142-C9CE-2E44-B771-9C3DBE8E6483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -713,6 +713,9 @@
                 <c:pt idx="149">
                   <c:v>44983</c:v>
                 </c:pt>
+                <c:pt idx="150">
+                  <c:v>44989</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1171,6 +1174,9 @@
                 </c:pt>
                 <c:pt idx="149">
                   <c:v>4784</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>4801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1668,6 +1674,9 @@
                 <c:pt idx="149">
                   <c:v>44983</c:v>
                 </c:pt>
+                <c:pt idx="150">
+                  <c:v>44989</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2126,6 +2135,9 @@
                 </c:pt>
                 <c:pt idx="149">
                   <c:v>3746</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>3750</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2625,6 +2637,9 @@
                 <c:pt idx="149">
                   <c:v>44983</c:v>
                 </c:pt>
+                <c:pt idx="150">
+                  <c:v>44989</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3083,6 +3098,9 @@
                 </c:pt>
                 <c:pt idx="149">
                   <c:v>549</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>562</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3601,6 +3619,9 @@
                 <c:pt idx="149">
                   <c:v>44983</c:v>
                 </c:pt>
+                <c:pt idx="150">
+                  <c:v>44989</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4058,6 +4079,9 @@
                   <c:v>477</c:v>
                 </c:pt>
                 <c:pt idx="149">
+                  <c:v>489</c:v>
+                </c:pt>
+                <c:pt idx="150">
                   <c:v>489</c:v>
                 </c:pt>
               </c:numCache>
@@ -4085,7 +4109,7 @@
         <c:axId val="1582352671"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="44990"/>
+          <c:max val="45000"/>
           <c:min val="44379"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -5286,13 +5310,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K152"/>
+  <dimension ref="A1:K153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B99" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I153" sqref="I153"/>
+      <selection pane="bottomRight" activeCell="N150" sqref="N150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10937,6 +10961,43 @@
         <v>549</v>
       </c>
       <c r="K152" s="7">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A153" s="1">
+        <v>44989</v>
+      </c>
+      <c r="B153" s="2">
+        <v>9</v>
+      </c>
+      <c r="C153">
+        <f t="shared" ref="C153" si="223">SUM(D153:F153)</f>
+        <v>1673</v>
+      </c>
+      <c r="D153">
+        <v>1105</v>
+      </c>
+      <c r="E153">
+        <v>371</v>
+      </c>
+      <c r="F153" s="3">
+        <v>197</v>
+      </c>
+      <c r="G153" s="4">
+        <v>52</v>
+      </c>
+      <c r="H153">
+        <f t="shared" ref="H153" si="224">SUM(I153:K153)</f>
+        <v>4801</v>
+      </c>
+      <c r="I153" s="5">
+        <v>3750</v>
+      </c>
+      <c r="J153" s="6">
+        <v>562</v>
+      </c>
+      <c r="K153" s="7">
         <v>489</v>
       </c>
     </row>
@@ -10958,7 +11019,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA10" sqref="AA10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Changed SectionHeader graphic in ReadmeView (from 8 to 7 boxes for iPad)
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA17142-C9CE-2E44-B771-9C3DBE8E6483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE33628-24C2-2D40-9BC6-F9725D2EFAA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -716,6 +716,9 @@
                 <c:pt idx="150">
                   <c:v>44989</c:v>
                 </c:pt>
+                <c:pt idx="151">
+                  <c:v>44990</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1177,6 +1180,9 @@
                 </c:pt>
                 <c:pt idx="150">
                   <c:v>4801</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>4826</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1677,6 +1683,9 @@
                 <c:pt idx="150">
                   <c:v>44989</c:v>
                 </c:pt>
+                <c:pt idx="151">
+                  <c:v>44990</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2138,6 +2147,9 @@
                 </c:pt>
                 <c:pt idx="150">
                   <c:v>3750</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>3778</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2640,6 +2652,9 @@
                 <c:pt idx="150">
                   <c:v>44989</c:v>
                 </c:pt>
+                <c:pt idx="151">
+                  <c:v>44990</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3101,6 +3116,9 @@
                 </c:pt>
                 <c:pt idx="150">
                   <c:v>562</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>564</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3622,6 +3640,9 @@
                 <c:pt idx="150">
                   <c:v>44989</c:v>
                 </c:pt>
+                <c:pt idx="151">
+                  <c:v>44990</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4083,6 +4104,9 @@
                 </c:pt>
                 <c:pt idx="150">
                   <c:v>489</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>484</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5310,13 +5334,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K153"/>
+  <dimension ref="A1:K154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B99" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N150" sqref="N150"/>
+      <selection pane="bottomRight" activeCell="G155" sqref="G155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10999,6 +11023,43 @@
       </c>
       <c r="K153" s="7">
         <v>489</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A154" s="1">
+        <v>44990</v>
+      </c>
+      <c r="B154" s="2">
+        <v>9</v>
+      </c>
+      <c r="C154">
+        <f t="shared" ref="C154" si="225">SUM(D154:F154)</f>
+        <v>1673</v>
+      </c>
+      <c r="D154">
+        <v>1105</v>
+      </c>
+      <c r="E154">
+        <v>371</v>
+      </c>
+      <c r="F154" s="3">
+        <v>197</v>
+      </c>
+      <c r="G154" s="4">
+        <v>53</v>
+      </c>
+      <c r="H154">
+        <f t="shared" ref="H154" si="226">SUM(I154:K154)</f>
+        <v>4826</v>
+      </c>
+      <c r="I154" s="5">
+        <v>3778</v>
+      </c>
+      <c r="J154" s="6">
+        <v>564</v>
+      </c>
+      <c r="K154" s="7">
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -11018,7 +11079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix: #144 Basic Roadmap support
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE33628-24C2-2D40-9BC6-F9725D2EFAA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AEF3ED-7F0E-5B4D-8824-E0E92AE28CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -719,6 +719,9 @@
                 <c:pt idx="151">
                   <c:v>44990</c:v>
                 </c:pt>
+                <c:pt idx="152">
+                  <c:v>44991</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1183,6 +1186,9 @@
                 </c:pt>
                 <c:pt idx="151">
                   <c:v>4826</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>4862</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1686,6 +1692,9 @@
                 <c:pt idx="151">
                   <c:v>44990</c:v>
                 </c:pt>
+                <c:pt idx="152">
+                  <c:v>44991</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2150,6 +2159,9 @@
                 </c:pt>
                 <c:pt idx="151">
                   <c:v>3778</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>3809</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2655,6 +2667,9 @@
                 <c:pt idx="151">
                   <c:v>44990</c:v>
                 </c:pt>
+                <c:pt idx="152">
+                  <c:v>44991</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3119,6 +3134,9 @@
                 </c:pt>
                 <c:pt idx="151">
                   <c:v>564</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>570</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3643,6 +3661,9 @@
                 <c:pt idx="151">
                   <c:v>44990</c:v>
                 </c:pt>
+                <c:pt idx="152">
+                  <c:v>44991</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4107,6 +4128,9 @@
                 </c:pt>
                 <c:pt idx="151">
                   <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5334,13 +5358,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K154"/>
+  <dimension ref="A1:K155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B99" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G155" sqref="G155"/>
+      <selection pane="bottomRight" activeCell="M155" sqref="M155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11060,6 +11084,43 @@
       </c>
       <c r="K154" s="7">
         <v>484</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A155" s="1">
+        <v>44991</v>
+      </c>
+      <c r="B155" s="2">
+        <v>9</v>
+      </c>
+      <c r="C155">
+        <f t="shared" ref="C155" si="227">SUM(D155:F155)</f>
+        <v>1673</v>
+      </c>
+      <c r="D155">
+        <v>1105</v>
+      </c>
+      <c r="E155">
+        <v>371</v>
+      </c>
+      <c r="F155" s="3">
+        <v>197</v>
+      </c>
+      <c r="G155" s="4">
+        <v>53</v>
+      </c>
+      <c r="H155">
+        <f t="shared" ref="H155" si="228">SUM(I155:K155)</f>
+        <v>4862</v>
+      </c>
+      <c r="I155" s="5">
+        <v>3809</v>
+      </c>
+      <c r="J155" s="6">
+        <v>570</v>
+      </c>
+      <c r="K155" s="7">
+        <v>483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: #153. Cleaned up VoteOnRoadmapView
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F9E0BD-FBA2-8040-BAA4-DF1A92A7E300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78AAD03-3A40-544A-93E7-A2D34FD2C2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -725,6 +725,9 @@
                 <c:pt idx="153">
                   <c:v>44992</c:v>
                 </c:pt>
+                <c:pt idx="154">
+                  <c:v>44996</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1195,6 +1198,9 @@
                 </c:pt>
                 <c:pt idx="153">
                   <c:v>4872</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>4899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1704,6 +1710,9 @@
                 <c:pt idx="153">
                   <c:v>44992</c:v>
                 </c:pt>
+                <c:pt idx="154">
+                  <c:v>44996</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2174,6 +2183,9 @@
                 </c:pt>
                 <c:pt idx="153">
                   <c:v>3823</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>3853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2685,6 +2697,9 @@
                 <c:pt idx="153">
                   <c:v>44992</c:v>
                 </c:pt>
+                <c:pt idx="154">
+                  <c:v>44996</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3154,6 +3169,9 @@
                   <c:v>570</c:v>
                 </c:pt>
                 <c:pt idx="153">
+                  <c:v>564</c:v>
+                </c:pt>
+                <c:pt idx="154">
                   <c:v>564</c:v>
                 </c:pt>
               </c:numCache>
@@ -3685,6 +3703,9 @@
                 <c:pt idx="153">
                   <c:v>44992</c:v>
                 </c:pt>
+                <c:pt idx="154">
+                  <c:v>44996</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4155,6 +4176,9 @@
                 </c:pt>
                 <c:pt idx="153">
                   <c:v>485</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>482</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5382,13 +5406,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K156"/>
+  <dimension ref="A1:K157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B99" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I157" sqref="I157"/>
+      <selection pane="bottomRight" activeCell="I158" sqref="I158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11182,6 +11206,43 @@
       </c>
       <c r="K156" s="7">
         <v>485</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A157" s="1">
+        <v>44996</v>
+      </c>
+      <c r="B157" s="2">
+        <v>9</v>
+      </c>
+      <c r="C157">
+        <f t="shared" ref="C157" si="231">SUM(D157:F157)</f>
+        <v>1673</v>
+      </c>
+      <c r="D157">
+        <v>1105</v>
+      </c>
+      <c r="E157">
+        <v>371</v>
+      </c>
+      <c r="F157" s="3">
+        <v>197</v>
+      </c>
+      <c r="G157" s="4">
+        <v>53</v>
+      </c>
+      <c r="H157">
+        <f t="shared" ref="H157" si="232">SUM(I157:K157)</f>
+        <v>4899</v>
+      </c>
+      <c r="I157" s="5">
+        <v>3853</v>
+      </c>
+      <c r="J157" s="6">
+        <v>564</v>
+      </c>
+      <c r="K157" s="7">
+        <v>482</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: #155. Cleanup button "Vote on roadmap items"
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78AAD03-3A40-544A-93E7-A2D34FD2C2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CB58C4-2793-2A4C-947B-AB71A7742471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="880" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -728,6 +728,9 @@
                 <c:pt idx="154">
                   <c:v>44996</c:v>
                 </c:pt>
+                <c:pt idx="155">
+                  <c:v>44997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1201,6 +1204,9 @@
                 </c:pt>
                 <c:pt idx="154">
                   <c:v>4899</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>4914</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1713,6 +1719,9 @@
                 <c:pt idx="154">
                   <c:v>44996</c:v>
                 </c:pt>
+                <c:pt idx="155">
+                  <c:v>44997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2186,6 +2195,9 @@
                 </c:pt>
                 <c:pt idx="154">
                   <c:v>3853</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>3865</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2700,6 +2712,9 @@
                 <c:pt idx="154">
                   <c:v>44996</c:v>
                 </c:pt>
+                <c:pt idx="155">
+                  <c:v>44997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3172,6 +3187,9 @@
                   <c:v>564</c:v>
                 </c:pt>
                 <c:pt idx="154">
+                  <c:v>564</c:v>
+                </c:pt>
+                <c:pt idx="155">
                   <c:v>564</c:v>
                 </c:pt>
               </c:numCache>
@@ -3706,6 +3724,9 @@
                 <c:pt idx="154">
                   <c:v>44996</c:v>
                 </c:pt>
+                <c:pt idx="155">
+                  <c:v>44997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4179,6 +4200,9 @@
                 </c:pt>
                 <c:pt idx="154">
                   <c:v>482</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>485</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5406,13 +5430,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K157"/>
+  <dimension ref="A1:K158"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B99" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I158" sqref="I158"/>
+      <selection pane="bottomRight" activeCell="N151" sqref="N151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11243,6 +11267,43 @@
       </c>
       <c r="K157" s="7">
         <v>482</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A158" s="1">
+        <v>44997</v>
+      </c>
+      <c r="B158" s="2">
+        <v>9</v>
+      </c>
+      <c r="C158">
+        <f t="shared" ref="C158" si="233">SUM(D158:F158)</f>
+        <v>1673</v>
+      </c>
+      <c r="D158">
+        <v>1105</v>
+      </c>
+      <c r="E158">
+        <v>371</v>
+      </c>
+      <c r="F158" s="3">
+        <v>197</v>
+      </c>
+      <c r="G158" s="4">
+        <v>53</v>
+      </c>
+      <c r="H158">
+        <f t="shared" ref="H158" si="234">SUM(I158:K158)</f>
+        <v>4914</v>
+      </c>
+      <c r="I158" s="5">
+        <v>3865</v>
+      </c>
+      <c r="J158" s="6">
+        <v>564</v>
+      </c>
+      <c r="K158" s="7">
+        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -11262,7 +11323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Reduced logging using ifDebugMode(String)
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25D2366-891C-A44E-A5AC-263FF0A1E5BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BD4A69-00F3-4B4E-AF59-F25FFF64EEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -737,6 +737,9 @@
                 <c:pt idx="157">
                   <c:v>45006</c:v>
                 </c:pt>
+                <c:pt idx="158">
+                  <c:v>45007</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1219,6 +1222,9 @@
                 </c:pt>
                 <c:pt idx="157">
                   <c:v>4940</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1739,6 +1745,9 @@
                 </c:pt>
                 <c:pt idx="157">
                   <c:v>45006</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>45007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2744,6 +2753,9 @@
                 </c:pt>
                 <c:pt idx="157">
                   <c:v>45006</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>45007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3769,6 +3781,9 @@
                 <c:pt idx="157">
                   <c:v>45006</c:v>
                 </c:pt>
+                <c:pt idx="158">
+                  <c:v>45007</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4314,7 +4329,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -5479,13 +5494,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K160"/>
+  <dimension ref="A1:K161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B99" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I161" sqref="I161"/>
+      <selection pane="bottomRight" activeCell="M157" sqref="M157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11427,6 +11442,34 @@
       </c>
       <c r="K160" s="7">
         <v>487</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A161" s="1">
+        <v>45007</v>
+      </c>
+      <c r="B161" s="2">
+        <v>9</v>
+      </c>
+      <c r="C161">
+        <f t="shared" ref="C161" si="239">SUM(D161:F161)</f>
+        <v>1673</v>
+      </c>
+      <c r="D161">
+        <v>1105</v>
+      </c>
+      <c r="E161">
+        <v>371</v>
+      </c>
+      <c r="F161" s="3">
+        <v>197</v>
+      </c>
+      <c r="G161" s="4">
+        <v>57</v>
+      </c>
+      <c r="H161">
+        <f t="shared" ref="H161" si="240">SUM(I161:K161)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to Readme screen's texts.
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D262EDD-94E4-7C44-8B82-19D7AE75A7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C080A8-5668-9E45-8001-17D136C0A2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -740,6 +740,9 @@
                 <c:pt idx="158">
                   <c:v>45007</c:v>
                 </c:pt>
+                <c:pt idx="159">
+                  <c:v>45008</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1225,6 +1228,9 @@
                 </c:pt>
                 <c:pt idx="158">
                   <c:v>4954</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>4931</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1749,6 +1755,9 @@
                 <c:pt idx="158">
                   <c:v>45007</c:v>
                 </c:pt>
+                <c:pt idx="159">
+                  <c:v>45008</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2234,6 +2243,9 @@
                 </c:pt>
                 <c:pt idx="158">
                   <c:v>3895</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>3888</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2760,6 +2772,9 @@
                 <c:pt idx="158">
                   <c:v>45007</c:v>
                 </c:pt>
+                <c:pt idx="159">
+                  <c:v>45008</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3245,6 +3260,9 @@
                 </c:pt>
                 <c:pt idx="158">
                   <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>560</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3790,6 +3808,9 @@
                 <c:pt idx="158">
                   <c:v>45007</c:v>
                 </c:pt>
+                <c:pt idx="159">
+                  <c:v>45008</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4275,6 +4296,9 @@
                 </c:pt>
                 <c:pt idx="158">
                   <c:v>489</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5503,13 +5527,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K161"/>
+  <dimension ref="A1:K162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B99" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M154" sqref="M154"/>
+      <selection pane="bottomRight" activeCell="I163" sqref="I163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11488,6 +11512,43 @@
       </c>
       <c r="K161" s="7">
         <v>489</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A162" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B162" s="2">
+        <v>9</v>
+      </c>
+      <c r="C162">
+        <f t="shared" ref="C162" si="241">SUM(D162:F162)</f>
+        <v>1673</v>
+      </c>
+      <c r="D162">
+        <v>1105</v>
+      </c>
+      <c r="E162">
+        <v>371</v>
+      </c>
+      <c r="F162" s="3">
+        <v>197</v>
+      </c>
+      <c r="G162" s="4">
+        <v>56</v>
+      </c>
+      <c r="H162">
+        <f t="shared" ref="H162" si="242">SUM(I162:K162)</f>
+        <v>4931</v>
+      </c>
+      <c r="I162" s="5">
+        <v>3888</v>
+      </c>
+      <c r="J162" s="6">
+        <v>560</v>
+      </c>
+      <c r="K162" s="7">
+        <v>483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Loading of TestPhotoClub Den Haag working in background.
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4758B06B-DD44-4643-A843-5FF4AF51FE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2ADA3F-C7D7-3241-A807-545CDEFDE920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
@@ -752,6 +752,9 @@
                 <c:pt idx="162">
                   <c:v>45117</c:v>
                 </c:pt>
+                <c:pt idx="163">
+                  <c:v>45127</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1249,6 +1252,9 @@
                 </c:pt>
                 <c:pt idx="162">
                   <c:v>4949</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>4406</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1785,6 +1791,9 @@
                 <c:pt idx="162">
                   <c:v>45117</c:v>
                 </c:pt>
+                <c:pt idx="163">
+                  <c:v>45127</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2282,6 +2291,9 @@
                 </c:pt>
                 <c:pt idx="162">
                   <c:v>3890</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>3577</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2820,6 +2832,9 @@
                 <c:pt idx="162">
                   <c:v>45117</c:v>
                 </c:pt>
+                <c:pt idx="163">
+                  <c:v>45127</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3317,6 +3332,9 @@
                 </c:pt>
                 <c:pt idx="162">
                   <c:v>571</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>435</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3874,6 +3892,9 @@
                 <c:pt idx="162">
                   <c:v>45117</c:v>
                 </c:pt>
+                <c:pt idx="163">
+                  <c:v>45127</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4371,6 +4392,9 @@
                 </c:pt>
                 <c:pt idx="162">
                   <c:v>488</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>394</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5599,13 +5623,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K165"/>
+  <dimension ref="A1:K166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B116" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I166" sqref="I166"/>
+      <selection pane="bottomRight" activeCell="I167" sqref="I167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11732,6 +11756,43 @@
       </c>
       <c r="K165" s="7">
         <v>488</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A166" s="1">
+        <v>45127</v>
+      </c>
+      <c r="B166" s="2">
+        <v>9</v>
+      </c>
+      <c r="C166">
+        <f t="shared" ref="C166" si="248">SUM(D166:F166)</f>
+        <v>1673</v>
+      </c>
+      <c r="D166">
+        <v>1105</v>
+      </c>
+      <c r="E166">
+        <v>371</v>
+      </c>
+      <c r="F166" s="3">
+        <v>197</v>
+      </c>
+      <c r="G166" s="4">
+        <v>56</v>
+      </c>
+      <c r="H166">
+        <f t="shared" ref="H166" si="249">SUM(I166:K166)</f>
+        <v>4406</v>
+      </c>
+      <c r="I166" s="5">
+        <v>3577</v>
+      </c>
+      <c r="J166" s="6">
+        <v>435</v>
+      </c>
+      <c r="K166" s="7">
+        <v>394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved code to new file insertOnlineMemberData as counterpart to insertSomeHardcodedMemberData
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F450DEFB-A106-D04D-8B61-BF54F65F7783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E0384E-7842-2E45-98EC-EC779068ED28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -5673,11 +5673,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
   <dimension ref="A1:K168"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B116" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I169" sqref="I169"/>
+      <selection pane="bottomRight" activeCell="G169" sqref="G169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11901,7 +11901,7 @@
         <v>197</v>
       </c>
       <c r="G168" s="4">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H168">
         <f t="shared" ref="H168" si="253">SUM(I168:K168)</f>
@@ -11934,7 +11934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA29" sqref="AA29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Replaced NSSortDescriptor by Sort Descriptor in Photographer.swift
</commit_message>
<xml_diff>
--- a/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
+++ b/Fotogroep Waalre/Documentation/FotogroepWaalre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Fotogroep Waalre 2/Fotogroep Waalre/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538A78FB-6883-6042-B8B9-69071B12D307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D6F07A-0317-6D44-8091-16D138231B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" activeTab="1" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="35220" windowHeight="26440" xr2:uid="{1D5C550A-6212-F143-B3FD-423F82763F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -770,6 +770,9 @@
                 <c:pt idx="168">
                   <c:v>45142</c:v>
                 </c:pt>
+                <c:pt idx="169">
+                  <c:v>45145</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1285,6 +1288,9 @@
                 </c:pt>
                 <c:pt idx="168">
                   <c:v>5112</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>5101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1839,6 +1845,9 @@
                 <c:pt idx="168">
                   <c:v>45142</c:v>
                 </c:pt>
+                <c:pt idx="169">
+                  <c:v>45145</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2354,6 +2363,9 @@
                 </c:pt>
                 <c:pt idx="168">
                   <c:v>4073</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>4063</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2910,6 +2922,9 @@
                 <c:pt idx="168">
                   <c:v>45142</c:v>
                 </c:pt>
+                <c:pt idx="169">
+                  <c:v>45145</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3424,6 +3439,9 @@
                   <c:v>571</c:v>
                 </c:pt>
                 <c:pt idx="168">
+                  <c:v>564</c:v>
+                </c:pt>
+                <c:pt idx="169">
                   <c:v>564</c:v>
                 </c:pt>
               </c:numCache>
@@ -4000,6 +4018,9 @@
                 <c:pt idx="168">
                   <c:v>45142</c:v>
                 </c:pt>
+                <c:pt idx="169">
+                  <c:v>45145</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4515,6 +4536,9 @@
                 </c:pt>
                 <c:pt idx="168">
                   <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>474</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5743,13 +5767,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E993F-B784-7448-B38E-9BEFCF4E7032}">
-  <dimension ref="A1:K171"/>
+  <dimension ref="A1:K172"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B116" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I172" sqref="I172"/>
+      <selection pane="bottomRight" activeCell="I173" sqref="I173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12098,6 +12122,43 @@
       </c>
       <c r="K171" s="7">
         <v>475</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A172" s="1">
+        <v>45145</v>
+      </c>
+      <c r="B172" s="2">
+        <v>9</v>
+      </c>
+      <c r="C172">
+        <f t="shared" ref="C172" si="260">SUM(D172:F172)</f>
+        <v>1673</v>
+      </c>
+      <c r="D172">
+        <v>1105</v>
+      </c>
+      <c r="E172">
+        <v>371</v>
+      </c>
+      <c r="F172" s="3">
+        <v>197</v>
+      </c>
+      <c r="G172" s="4">
+        <v>58</v>
+      </c>
+      <c r="H172">
+        <f t="shared" ref="H172" si="261">SUM(I172:K172)</f>
+        <v>5101</v>
+      </c>
+      <c r="I172" s="5">
+        <v>4063</v>
+      </c>
+      <c r="J172" s="6">
+        <v>564</v>
+      </c>
+      <c r="K172" s="7">
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -12117,7 +12178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E980CBD7-53A1-DE45-BAAC-5516721A0BEE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA29" sqref="AA29"/>
     </sheetView>
   </sheetViews>

</xml_diff>